<commit_message>
Magnetic Design Excel Updated Source Documents Added
</commit_message>
<xml_diff>
--- a/Magnetic Design/Transformer_Design_Excel.xlsx
+++ b/Magnetic Design/Transformer_Design_Excel.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahmetcan.akuz\Documents\GitHub\Optimus-Primary-Winding\Magnetic Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E03A2A3D-99A1-44EA-B706-18BFB1F8C212}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01874644-CDB1-4449-A2F1-228A6FF433FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19110" yWindow="0" windowWidth="19380" windowHeight="20970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="42">
   <si>
     <t>Voltage Pri Min</t>
   </si>
@@ -141,6 +142,27 @@
   </si>
   <si>
     <t>Ns_integer</t>
+  </si>
+  <si>
+    <t>L_sec</t>
+  </si>
+  <si>
+    <t>Isec</t>
+  </si>
+  <si>
+    <t>Isec,rms</t>
+  </si>
+  <si>
+    <t>primary inductance</t>
+  </si>
+  <si>
+    <t>secondary inductance</t>
+  </si>
+  <si>
+    <t>primary turn</t>
+  </si>
+  <si>
+    <t>secondary turn</t>
   </si>
 </sst>
 </file>
@@ -195,7 +217,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -330,18 +352,43 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -351,7 +398,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -361,7 +407,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -374,7 +419,18 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Check Cell" xfId="1" builtinId="23"/>
@@ -404,9 +460,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>324039</xdr:colOff>
+      <xdr:colOff>263079</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>26450</xdr:rowOff>
+      <xdr:rowOff>35340</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -451,9 +507,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>224350</xdr:colOff>
+      <xdr:colOff>225620</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>163591</xdr:rowOff>
+      <xdr:rowOff>155971</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -495,9 +551,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>453584</xdr:colOff>
+      <xdr:colOff>377384</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>100607</xdr:rowOff>
+      <xdr:rowOff>110767</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -541,7 +597,7 @@
       <xdr:col>18</xdr:col>
       <xdr:colOff>224963</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>108227</xdr:rowOff>
+      <xdr:rowOff>110767</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -583,9 +639,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>26183</xdr:colOff>
+      <xdr:colOff>35073</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>160934</xdr:rowOff>
+      <xdr:rowOff>155854</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -629,7 +685,7 @@
       <xdr:col>15</xdr:col>
       <xdr:colOff>79509</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>128764</xdr:rowOff>
+      <xdr:rowOff>117334</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -671,9 +727,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>141136</xdr:colOff>
+      <xdr:colOff>148756</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>89697</xdr:rowOff>
+      <xdr:rowOff>79537</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -702,6 +758,85 @@
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>141947</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>463550</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>60959</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9461F175-48CB-0DAE-B05C-F81C8BC77CF5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="510247"/>
+          <a:ext cx="14484350" cy="6732562"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -972,27 +1107,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P26"/>
+  <dimension ref="A1:P34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N6" sqref="N6"/>
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.44140625" customWidth="1"/>
-    <col min="4" max="4" width="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="4.6640625" customWidth="1"/>
+    <col min="7" max="7" width="10.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="6"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="9"/>
     </row>
     <row r="2" spans="1:16" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
@@ -1041,7 +1177,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="1">
-        <v>50000</v>
+        <v>60000</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>7</v>
@@ -1063,7 +1199,7 @@
       <c r="A8" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="16">
+      <c r="B8" s="6">
         <v>1</v>
       </c>
       <c r="C8" s="1" t="s">
@@ -1080,30 +1216,30 @@
       <c r="C9" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F9" s="7" t="s">
+      <c r="F9" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="G9" s="15" t="s">
+      <c r="G9" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="H9" s="15"/>
-      <c r="I9" s="15"/>
-      <c r="J9" s="15"/>
+      <c r="H9" s="16"/>
+      <c r="I9" s="16"/>
+      <c r="J9" s="16"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A10" s="11"/>
+      <c r="A10" s="5"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A11" s="8" t="s">
+      <c r="A11" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="9"/>
-      <c r="C11" s="10"/>
+      <c r="B11" s="11"/>
+      <c r="C11" s="12"/>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="4" t="s">
         <v>12</v>
       </c>
       <c r="B12" s="1">
@@ -1115,7 +1251,7 @@
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="4" t="s">
         <v>14</v>
       </c>
       <c r="B13" s="1">
@@ -1127,7 +1263,7 @@
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A14" s="7" t="s">
+      <c r="A14" s="4" t="s">
         <v>11</v>
       </c>
       <c r="B14" s="1">
@@ -1149,7 +1285,7 @@
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A15" s="7" t="s">
+      <c r="A15" s="4" t="s">
         <v>25</v>
       </c>
       <c r="B15" s="1">
@@ -1161,16 +1297,16 @@
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A16" s="7"/>
+      <c r="A16" s="4"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A17" s="12" t="s">
+      <c r="A17" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="13"/>
-      <c r="C17" s="14"/>
+      <c r="B17" s="14"/>
+      <c r="C17" s="15"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
@@ -1196,8 +1332,8 @@
       <c r="A19" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B19" s="16">
-        <v>54</v>
+      <c r="B19" s="6">
+        <v>81</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>24</v>
@@ -1207,44 +1343,52 @@
       <c r="A20" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B20" s="16">
-        <v>50</v>
+      <c r="B20" s="6">
+        <v>151</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A21" s="7" t="s">
+      <c r="A21" s="4" t="s">
         <v>27</v>
       </c>
       <c r="B21" s="1">
         <f>(B2*B14)/(B13*B6)</f>
-        <v>6.3749999999999999E-6</v>
+        <v>5.3124999999999995E-6</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>30</v>
       </c>
       <c r="D21" s="1">
         <f>B21*1000000</f>
-        <v>6.375</v>
+        <v>5.3124999999999991</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>31</v>
       </c>
+      <c r="F21" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="G21" s="21"/>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A22" s="7" t="s">
+      <c r="A22" s="4" t="s">
         <v>29</v>
       </c>
       <c r="B22" s="1">
         <f>(B21*B13*10^6)/(B18*B19)</f>
-        <v>7.4074074074074074</v>
+        <v>4.1152263374485587</v>
       </c>
       <c r="C22" s="1"/>
+      <c r="F22" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="G22" s="19"/>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A23" s="7" t="s">
+      <c r="A23" s="4" t="s">
         <v>28</v>
       </c>
       <c r="B23" s="1">
@@ -1254,42 +1398,115 @@
       <c r="C23" s="1"/>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A24" s="7" t="s">
+      <c r="A24" s="4" t="s">
         <v>32</v>
       </c>
       <c r="B24" s="1">
         <f>ROUND(B22,0)</f>
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C24" s="1"/>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A25" s="7" t="s">
+      <c r="A25" s="4" t="s">
         <v>33</v>
       </c>
       <c r="B25" s="1">
         <f>B24/B23</f>
-        <v>28.583333333333336</v>
+        <v>16.333333333333332</v>
       </c>
       <c r="C25" s="1"/>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A26" s="7" t="s">
+      <c r="A26" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="B26" s="1">
+      <c r="B26" s="18">
         <f>ROUND(B25,0)</f>
-        <v>29</v>
-      </c>
-      <c r="C26" s="1"/>
+        <v>16</v>
+      </c>
+      <c r="C26" s="18"/>
+      <c r="F26" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="G26" s="19"/>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A27" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B27" s="1">
+        <f>B21*(B23)^2</f>
+        <v>3.1861724281549349E-7</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D27" s="1">
+        <f>B27*1000000</f>
+        <v>0.31861724281549347</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F27" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="G27" s="21"/>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A28" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B28" s="1">
+        <f>B13*B24/B26</f>
+        <v>4.7058823529411766</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A29" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B29" s="1">
+        <f>B28*SQRT((1-B14)/3)</f>
+        <v>1.9211684257122965</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="34" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D34" s="22"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="8">
+    <mergeCell ref="F27:G27"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="F22:G22"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A11:C11"/>
     <mergeCell ref="A17:C17"/>
     <mergeCell ref="G9:J9"/>
+    <mergeCell ref="F26:G26"/>
   </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EE355BF-C773-4D1D-B00A-4E91F8B61265}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -1300,7 +1517,7 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{41977015-9153-4136-90D6-F1BDBE157B07}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D7965DE1-26C6-497C-B995-A19305410089}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
     <ds:schemaRef ds:uri="http://www.boldonjames.com/2008/01/sie/internal/label"/>

</xml_diff>

<commit_message>
Magnetic Design Updated wrt CCM Mode
</commit_message>
<xml_diff>
--- a/Magnetic Design/Transformer_Design_Excel.xlsx
+++ b/Magnetic Design/Transformer_Design_Excel.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahmetcan.akuz\Documents\GitHub\EE464_2022_HW1_Team5\Magnetic_Design\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahmetcan.akuz\Documents\GitHub\Optimus-Primary-Winding\Magnetic Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35BDCD9A-8EF0-426A-81C1-7943753B568B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA21A692-B64F-436E-A033-26A1FE22BB66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12910" yWindow="8160" windowWidth="22930" windowHeight="12410" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-90" yWindow="0" windowWidth="19380" windowHeight="20970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -150,7 +150,7 @@
     <t>Isec,rms</t>
   </si>
   <si>
-    <t>magnetizing inductance</t>
+    <t>Kf</t>
   </si>
 </sst>
 </file>
@@ -367,7 +367,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -381,9 +381,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
@@ -416,6 +413,8 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Check Cell" xfId="1" builtinId="23"/>
@@ -445,7 +444,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>180529</xdr:colOff>
+      <xdr:colOff>186879</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>35340</xdr:rowOff>
     </xdr:to>
@@ -529,50 +528,6 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>281940</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>60960</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>294834</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>110767</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EA855D38-1739-4528-9BCE-C73623DB5349}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6484620" y="3009900"/>
-          <a:ext cx="1390844" cy="405407"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
       <xdr:col>16</xdr:col>
       <xdr:colOff>205740</xdr:colOff>
       <xdr:row>12</xdr:row>
@@ -598,7 +553,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -642,7 +597,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -651,50 +606,6 @@
         <a:xfrm>
           <a:off x="8823960" y="3063240"/>
           <a:ext cx="1062503" cy="412394"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>350520</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>111981</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>79509</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>117334</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="7" name="Picture 6">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3D20FED0-0F01-41AE-AF78-3EC282A3B146}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="10820400" y="3060921"/>
-          <a:ext cx="948189" cy="382543"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -730,7 +641,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -739,6 +650,94 @@
         <a:xfrm>
           <a:off x="10629900" y="2316480"/>
           <a:ext cx="1200316" cy="356397"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>339090</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>115570</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>415388</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>148611</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Picture 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{901BB1FA-F107-1B26-59E1-9CF1E13FEDF3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9159240" y="3081020"/>
+          <a:ext cx="1897478" cy="401341"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>135890</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>144780</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>273128</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>116877</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Picture 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E46A4CA8-430C-C118-8B6D-96DA8EBF878A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4530090" y="2926080"/>
+          <a:ext cx="1517728" cy="709967"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1094,28 +1093,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26:G26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H35" sqref="H35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.08984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.453125" customWidth="1"/>
+    <col min="2" max="2" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.44140625" customWidth="1"/>
     <col min="4" max="4" width="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="4.6328125" customWidth="1"/>
-    <col min="7" max="7" width="11.26953125" customWidth="1"/>
+    <col min="5" max="5" width="4.6640625" customWidth="1"/>
+    <col min="7" max="7" width="11.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:16" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="14"/>
-    </row>
-    <row r="2" spans="1:16" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="B1" s="12"/>
+      <c r="C1" s="13"/>
+    </row>
+    <row r="2" spans="1:16" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1126,7 +1125,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -1137,7 +1136,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -1148,16 +1147,16 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="1">
-        <v>0.9</v>
+        <v>0.85</v>
       </c>
       <c r="C5" s="1"/>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
@@ -1168,7 +1167,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
@@ -1180,7 +1179,7 @@
       </c>
       <c r="K7" s="3"/>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>16</v>
       </c>
@@ -1191,12 +1190,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B9" s="1">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>1</v>
@@ -1204,56 +1203,60 @@
       <c r="F9" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="G9" s="21" t="s">
+      <c r="G9" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="H9" s="21"/>
-      <c r="I9" s="21"/>
-      <c r="J9" s="21"/>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A10" s="5"/>
-      <c r="B10" s="1"/>
+      <c r="H9" s="20"/>
+      <c r="I9" s="20"/>
+      <c r="J9" s="20"/>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A10" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" s="1">
+        <v>0.4</v>
+      </c>
       <c r="C10" s="1"/>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A11" s="15" t="s">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A11" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="16"/>
-      <c r="C11" s="17"/>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="B11" s="15"/>
+      <c r="C11" s="16"/>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>12</v>
       </c>
       <c r="B12" s="1">
         <f>B4/B5</f>
-        <v>53.333333333333329</v>
+        <v>56.470588235294116</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>14</v>
       </c>
       <c r="B13" s="1">
         <f>2*B12/(B2*B14)</f>
-        <v>14.814814814814815</v>
+        <v>18.823529411764707</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>11</v>
       </c>
       <c r="B14" s="6">
         <f>B9/(B9+B2)</f>
-        <v>0.6</v>
+        <v>0.5</v>
       </c>
       <c r="C14" s="6"/>
       <c r="F14">
@@ -1269,31 +1272,31 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>25</v>
       </c>
       <c r="B15" s="1">
         <f>B13*SQRT(B14/3)</f>
-        <v>6.6253865999993771</v>
+        <v>7.684673702849186</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16" s="4"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A17" s="18" t="s">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A17" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="19"/>
-      <c r="C17" s="20"/>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="B17" s="18"/>
+      <c r="C17" s="19"/>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>20</v>
       </c>
@@ -1313,7 +1316,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>21</v>
       </c>
@@ -1324,7 +1327,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>22</v>
       </c>
@@ -1335,115 +1338,112 @@
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
         <v>27</v>
       </c>
       <c r="B21" s="1">
-        <f>(B2*B14)/(B13*B6)</f>
-        <v>8.0999999999999987E-6</v>
+        <f>(B2*B14)^2/(2*B12*B6*B10)</f>
+        <v>1.3281250000000001E-5</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>30</v>
       </c>
       <c r="D21" s="1">
         <f>B21*1000000</f>
-        <v>8.0999999999999979</v>
+        <v>13.281250000000002</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="F21" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="G21" s="10"/>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="F21" s="21"/>
+      <c r="G21" s="22"/>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
         <v>29</v>
       </c>
       <c r="B22" s="1">
         <f>(B21*B13*10^6)/(B18*B19)</f>
-        <v>4.9382716049382704</v>
+        <v>10.288065843621398</v>
       </c>
       <c r="C22" s="1"/>
-      <c r="F22" s="10"/>
-      <c r="G22" s="10"/>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="F22" s="22"/>
+      <c r="G22" s="22"/>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
         <v>28</v>
       </c>
       <c r="B23" s="1">
-        <f>B9/(B7+B8)</f>
-        <v>0.36734693877551022</v>
+        <f>(B2*B14)/((B4+B8)*(1-B14))</f>
+        <v>0.24489795918367346</v>
       </c>
       <c r="C23" s="1"/>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
         <v>32</v>
       </c>
       <c r="B24" s="1">
         <f>ROUND(B22,0)</f>
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C24" s="1"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
         <v>33</v>
       </c>
       <c r="B25" s="1">
         <f>B24/B23</f>
-        <v>13.611111111111111</v>
+        <v>40.833333333333336</v>
       </c>
       <c r="C25" s="1"/>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26" s="7" t="s">
         <v>34</v>
       </c>
       <c r="B26" s="8">
         <f>ROUND(B25,0)</f>
-        <v>14</v>
+        <v>41</v>
       </c>
       <c r="C26" s="8"/>
       <c r="F26" s="10"/>
       <c r="G26" s="10"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
         <v>35</v>
       </c>
       <c r="B27" s="1">
         <f>B13*B24/B26</f>
-        <v>5.2910052910052912</v>
+        <v>4.5911047345767582</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
         <v>36</v>
       </c>
       <c r="B28" s="1">
         <f>B27*SQRT((1-B14)/3)</f>
-        <v>1.9320019665085224</v>
+        <v>1.8743106592315091</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="33" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="33" spans="4:6" x14ac:dyDescent="0.3">
       <c r="D33" s="9"/>
+      <c r="F33" s="9"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="5">
     <mergeCell ref="F26:G26"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="F22:G22"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A11:C11"/>
     <mergeCell ref="A17:C17"/>
@@ -1462,7 +1462,7 @@
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -1474,7 +1474,7 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9FB36A01-E898-4B1C-B19D-85961DA364E3}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7BCF8C47-8241-4988-BB65-BC89EC2C5C09}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
     <ds:schemaRef ds:uri="http://www.boldonjames.com/2008/01/sie/internal/label"/>

</xml_diff>

<commit_message>
Cable Selection Part was added.
</commit_message>
<xml_diff>
--- a/Magnetic Design/Transformer_Design_Excel.xlsx
+++ b/Magnetic Design/Transformer_Design_Excel.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahmetcan.akuz\Documents\GitHub\Optimus-Primary-Winding\Magnetic Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{365EDB9F-E937-4279-B2BD-AE4185DB71F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6FB5644-F5C0-432B-A38B-0DE993A57C5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="11364" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Transformer_Design" sheetId="1" r:id="rId1"/>
+    <sheet name="AWG" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,8 +37,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="141">
   <si>
     <t>Voltage Pri Min</t>
   </si>
@@ -168,17 +191,317 @@
     <t>Krf</t>
   </si>
   <si>
-    <t>Fill factor, Kf</t>
-  </si>
-  <si>
     <t>Window Area,Aw</t>
+  </si>
+  <si>
+    <t>A_pri</t>
+  </si>
+  <si>
+    <t>A_sec</t>
+  </si>
+  <si>
+    <t>Winding Area</t>
+  </si>
+  <si>
+    <t>Fill factor, Kcu</t>
+  </si>
+  <si>
+    <t>G gauge</t>
+  </si>
+  <si>
+    <t>Conductor</t>
+  </si>
+  <si>
+    <t>Diameter Inches</t>
+  </si>
+  <si>
+    <t>Diameter mm</t>
+  </si>
+  <si>
+    <r>
+      <t>Conductor cross section in mm</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>2</t>
+    </r>
+  </si>
+  <si>
+    <t>Ohms per 1000 ft.</t>
+  </si>
+  <si>
+    <t>Ohms per km</t>
+  </si>
+  <si>
+    <t>Maximum amps for chassis wiring</t>
+  </si>
+  <si>
+    <t>Maximum amps for</t>
+  </si>
+  <si>
+    <t>power transmission</t>
+  </si>
+  <si>
+    <t>Maximum frequency for</t>
+  </si>
+  <si>
+    <t>100% skin depth for solid conductor copper</t>
+  </si>
+  <si>
+    <t>Breaking force Soft Annealed Cu 37000 PSI</t>
+  </si>
+  <si>
+    <t>125 Hz</t>
+  </si>
+  <si>
+    <t>6120 lbs</t>
+  </si>
+  <si>
+    <t>160 Hz</t>
+  </si>
+  <si>
+    <t>4860 lbs</t>
+  </si>
+  <si>
+    <t>200 Hz</t>
+  </si>
+  <si>
+    <t>3860 lbs</t>
+  </si>
+  <si>
+    <t>250 Hz</t>
+  </si>
+  <si>
+    <t>3060 lbs</t>
+  </si>
+  <si>
+    <t>325 Hz</t>
+  </si>
+  <si>
+    <t>2430 lbs</t>
+  </si>
+  <si>
+    <t>410 Hz</t>
+  </si>
+  <si>
+    <t>1930 lbs</t>
+  </si>
+  <si>
+    <t>500 Hz</t>
+  </si>
+  <si>
+    <t>1530 lbs</t>
+  </si>
+  <si>
+    <t>650 Hz</t>
+  </si>
+  <si>
+    <t>1210 lbs</t>
+  </si>
+  <si>
+    <t>810 Hz</t>
+  </si>
+  <si>
+    <t>960 lbs</t>
+  </si>
+  <si>
+    <t>1100 Hz</t>
+  </si>
+  <si>
+    <t>760 lbs</t>
+  </si>
+  <si>
+    <t>1300 Hz</t>
+  </si>
+  <si>
+    <t>605 lbs</t>
+  </si>
+  <si>
+    <t>1650 Hz</t>
+  </si>
+  <si>
+    <t>480 lbs</t>
+  </si>
+  <si>
+    <t>2050 Hz</t>
+  </si>
+  <si>
+    <t>380 lbs</t>
+  </si>
+  <si>
+    <t>2600 Hz</t>
+  </si>
+  <si>
+    <t>314 lbs</t>
+  </si>
+  <si>
+    <t>3200 Hz</t>
+  </si>
+  <si>
+    <t>249 lbs</t>
+  </si>
+  <si>
+    <t>4150 Hz</t>
+  </si>
+  <si>
+    <t>197 lbs</t>
+  </si>
+  <si>
+    <t>5300 Hz</t>
+  </si>
+  <si>
+    <t>150 lbs</t>
+  </si>
+  <si>
+    <t>6700 Hz</t>
+  </si>
+  <si>
+    <t>119 lbs</t>
+  </si>
+  <si>
+    <t>8250 Hz</t>
+  </si>
+  <si>
+    <t>94 lbs</t>
+  </si>
+  <si>
+    <t>11 k Hz</t>
+  </si>
+  <si>
+    <t>75 lbs</t>
+  </si>
+  <si>
+    <t>13 k Hz</t>
+  </si>
+  <si>
+    <t>59 lbs</t>
+  </si>
+  <si>
+    <t>17 kHz</t>
+  </si>
+  <si>
+    <t>47 lbs</t>
+  </si>
+  <si>
+    <t>21 kHz</t>
+  </si>
+  <si>
+    <t>37 lbs</t>
+  </si>
+  <si>
+    <t>27 kHz</t>
+  </si>
+  <si>
+    <t>29 lbs</t>
+  </si>
+  <si>
+    <t>33 kHz</t>
+  </si>
+  <si>
+    <t>23 lbs</t>
+  </si>
+  <si>
+    <t>42 kHz</t>
+  </si>
+  <si>
+    <t>18 lbs</t>
+  </si>
+  <si>
+    <t>53 kHz</t>
+  </si>
+  <si>
+    <t>14.5 lbs</t>
+  </si>
+  <si>
+    <t>68 kHz</t>
+  </si>
+  <si>
+    <t>11.5 lbs</t>
+  </si>
+  <si>
+    <t>85 kHz</t>
+  </si>
+  <si>
+    <t>9 lbs</t>
+  </si>
+  <si>
+    <t>107 kHz</t>
+  </si>
+  <si>
+    <t>7.2 lbs</t>
+  </si>
+  <si>
+    <t>130 kHz</t>
+  </si>
+  <si>
+    <t>5.5 lbs</t>
+  </si>
+  <si>
+    <t>170 kHz</t>
+  </si>
+  <si>
+    <t>4.5 lbs</t>
+  </si>
+  <si>
+    <t>210 kHz</t>
+  </si>
+  <si>
+    <t>3.6 lbs</t>
+  </si>
+  <si>
+    <t>270 kHz</t>
+  </si>
+  <si>
+    <t>2.75 lbs</t>
+  </si>
+  <si>
+    <t>340 kHz</t>
+  </si>
+  <si>
+    <t>2.25 lbs</t>
+  </si>
+  <si>
+    <t>430 kHz</t>
+  </si>
+  <si>
+    <t>1.8 lbs</t>
+  </si>
+  <si>
+    <t>Metric 2.0</t>
+  </si>
+  <si>
+    <t>440 kHz</t>
+  </si>
+  <si>
+    <t>primary cable AWG</t>
+  </si>
+  <si>
+    <t>Diameter</t>
+  </si>
+  <si>
+    <t>secondary cable AWG</t>
+  </si>
+  <si>
+    <t>Area</t>
+  </si>
+  <si>
+    <t>Parallel</t>
+  </si>
+  <si>
+    <t>mm</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -194,8 +517,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <vertAlign val="superscript"/>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -225,8 +561,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFA9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="14">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -383,12 +725,66 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -401,6 +797,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -434,8 +831,30 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Check Cell" xfId="1" builtinId="23"/>
@@ -465,7 +884,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>186879</xdr:colOff>
+      <xdr:colOff>181799</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>35340</xdr:rowOff>
     </xdr:to>
@@ -514,7 +933,7 @@
       <xdr:col>12</xdr:col>
       <xdr:colOff>225620</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>155971</xdr:rowOff>
+      <xdr:rowOff>161051</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -556,9 +975,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>224963</xdr:colOff>
+      <xdr:colOff>219883</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>110767</xdr:rowOff>
+      <xdr:rowOff>105687</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -602,7 +1021,7 @@
       <xdr:col>12</xdr:col>
       <xdr:colOff>35073</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>155854</xdr:rowOff>
+      <xdr:rowOff>160934</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -644,9 +1063,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>148756</xdr:colOff>
+      <xdr:colOff>143676</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>79537</xdr:rowOff>
+      <xdr:rowOff>84617</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -688,9 +1107,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>415388</xdr:colOff>
+      <xdr:colOff>410308</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>148611</xdr:rowOff>
+      <xdr:rowOff>143531</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -732,7 +1151,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>273128</xdr:colOff>
+      <xdr:colOff>279478</xdr:colOff>
       <xdr:row>19</xdr:row>
       <xdr:rowOff>116877</xdr:rowOff>
     </xdr:to>
@@ -1112,28 +1531,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P33"/>
+  <dimension ref="A1:P37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="L31" sqref="L31"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.77734375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.44140625" customWidth="1"/>
     <col min="4" max="4" width="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="4.6640625" customWidth="1"/>
+    <col min="5" max="5" width="7.109375" customWidth="1"/>
     <col min="7" max="7" width="11.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="13"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="14"/>
     </row>
     <row r="2" spans="1:16" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
@@ -1224,15 +1643,15 @@
       <c r="F9" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="G9" s="20" t="s">
+      <c r="G9" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="H9" s="20"/>
-      <c r="I9" s="20"/>
-      <c r="J9" s="20"/>
+      <c r="H9" s="21"/>
+      <c r="I9" s="21"/>
+      <c r="J9" s="21"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A10" s="21" t="s">
+      <c r="A10" s="10" t="s">
         <v>42</v>
       </c>
       <c r="B10" s="1">
@@ -1241,11 +1660,11 @@
       <c r="C10" s="1"/>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A11" s="14" t="s">
+      <c r="A11" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="15"/>
-      <c r="C11" s="16"/>
+      <c r="B11" s="16"/>
+      <c r="C11" s="17"/>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
@@ -1311,11 +1730,11 @@
       <c r="C16" s="1"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A17" s="17" t="s">
+      <c r="A17" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="18"/>
-      <c r="C17" s="19"/>
+      <c r="B17" s="19"/>
+      <c r="C17" s="20"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
@@ -1342,7 +1761,7 @@
         <v>21</v>
       </c>
       <c r="B19" s="5">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>23</v>
@@ -1350,7 +1769,7 @@
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B20" s="5">
         <v>151</v>
@@ -1389,7 +1808,7 @@
         <v>30</v>
       </c>
       <c r="F22" s="9"/>
-      <c r="I22" s="1"/>
+      <c r="I22" s="31"/>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
@@ -1397,7 +1816,7 @@
       </c>
       <c r="B23" s="1">
         <f>(B22*B13*10^6)/(B18*B19)</f>
-        <v>10.288065843621398</v>
+        <v>9.9206349206349209</v>
       </c>
       <c r="C23" s="1"/>
     </row>
@@ -1440,8 +1859,8 @@
         <v>41</v>
       </c>
       <c r="C27" s="7"/>
-      <c r="F27" s="10"/>
-      <c r="G27" s="10"/>
+      <c r="F27" s="11"/>
+      <c r="G27" s="11"/>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
@@ -1473,7 +1892,7 @@
       </c>
       <c r="B30" s="1">
         <f>40*3.14*B19*((B23^2)/(1000*B23)+(1/B21))</f>
-        <v>174.34885844748857</v>
+        <v>176.92968036529683</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>39</v>
@@ -1484,22 +1903,127 @@
         <v>40</v>
       </c>
       <c r="B31" s="1">
-        <v>5</v>
-      </c>
-      <c r="C31" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="C31" s="1" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A32" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B32" s="1"/>
-      <c r="C32" s="1"/>
-    </row>
-    <row r="33" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D33" s="8"/>
-      <c r="F33" s="8"/>
+      <c r="A32" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B32" s="1">
+        <f>B15/B31</f>
+        <v>1.9211684257122965</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D32" s="8"/>
+      <c r="F32" s="8"/>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A33" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B33" s="1">
+        <f>B29/B31</f>
+        <v>0.46857766480787727</v>
+      </c>
+      <c r="C33" s="7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A34" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B34" s="1">
+        <v>24</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="D34" s="1" cm="1">
+        <f t="array" aca="1" ref="D34" ca="1">INDIRECT("AWG!D" &amp; B34+6)</f>
+        <v>0.20499999999999999</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F34" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="G34" s="30" cm="1">
+        <f t="array" aca="1" ref="G34" ca="1">INDIRECT("AWG!C" &amp; B34+6)</f>
+        <v>0.51053999999999999</v>
+      </c>
+      <c r="H34" s="30" t="s">
+        <v>140</v>
+      </c>
+      <c r="I34" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="J34" s="1">
+        <f ca="1">ROUNDUP(B32/D34,0)</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A35" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="B35" s="1">
+        <v>24</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="D35" s="1" cm="1">
+        <f t="array" aca="1" ref="D35" ca="1">INDIRECT("AWG!D" &amp; B34+6)</f>
+        <v>0.20499999999999999</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F35" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="G35" s="1" cm="1">
+        <f t="array" aca="1" ref="G35" ca="1">INDIRECT("AWG!C" &amp; B35+6)</f>
+        <v>0.51053999999999999</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="I35" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="J35" s="1">
+        <f ca="1">ROUNDUP(B33/D35,0)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A36" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B36" s="1">
+        <f>B32*B25+B27*B33</f>
+        <v>38.423368514245936</v>
+      </c>
+      <c r="C36" s="28"/>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A37" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B37" s="1">
+        <f>B36/B20</f>
+        <v>0.25445939413407903</v>
+      </c>
+      <c r="C37" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -1515,6 +2039,1268 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B96DE545-7F3F-4161-810A-0A86D0D5D381}">
+  <dimension ref="A1:J39"/>
+  <sheetViews>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="Q15" sqref="Q15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="7.21875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A1" s="26" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="C1" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1" s="26" t="s">
+        <v>52</v>
+      </c>
+      <c r="E1" s="26" t="s">
+        <v>53</v>
+      </c>
+      <c r="F1" s="26" t="s">
+        <v>54</v>
+      </c>
+      <c r="G1" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="H1" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="I1" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="J1" s="26" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="35.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="27"/>
+      <c r="B2" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" s="23" t="s">
+        <v>51</v>
+      </c>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="I2" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="J2" s="27"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" s="24">
+        <v>0</v>
+      </c>
+      <c r="B3" s="25">
+        <v>0.46</v>
+      </c>
+      <c r="C3" s="25">
+        <v>11.683999999999999</v>
+      </c>
+      <c r="D3" s="29">
+        <v>107</v>
+      </c>
+      <c r="E3" s="25">
+        <v>4.9000000000000002E-2</v>
+      </c>
+      <c r="F3" s="25">
+        <v>0.16072</v>
+      </c>
+      <c r="G3" s="25">
+        <v>380</v>
+      </c>
+      <c r="H3" s="25">
+        <v>302</v>
+      </c>
+      <c r="I3" s="25" t="s">
+        <v>61</v>
+      </c>
+      <c r="J3" s="25" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" s="24">
+        <v>0</v>
+      </c>
+      <c r="B4" s="25">
+        <v>0.40960000000000002</v>
+      </c>
+      <c r="C4" s="25">
+        <v>10.403840000000001</v>
+      </c>
+      <c r="D4" s="29">
+        <v>84.9</v>
+      </c>
+      <c r="E4" s="25">
+        <v>6.1800000000000001E-2</v>
+      </c>
+      <c r="F4" s="25">
+        <v>0.202704</v>
+      </c>
+      <c r="G4" s="25">
+        <v>328</v>
+      </c>
+      <c r="H4" s="25">
+        <v>239</v>
+      </c>
+      <c r="I4" s="25" t="s">
+        <v>63</v>
+      </c>
+      <c r="J4" s="25" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" s="24">
+        <v>0</v>
+      </c>
+      <c r="B5" s="25">
+        <v>0.36480000000000001</v>
+      </c>
+      <c r="C5" s="25">
+        <v>9.2659199999999995</v>
+      </c>
+      <c r="D5" s="29">
+        <v>67.400000000000006</v>
+      </c>
+      <c r="E5" s="25">
+        <v>7.7899999999999997E-2</v>
+      </c>
+      <c r="F5" s="25">
+        <v>0.25551200000000002</v>
+      </c>
+      <c r="G5" s="25">
+        <v>283</v>
+      </c>
+      <c r="H5" s="25">
+        <v>190</v>
+      </c>
+      <c r="I5" s="25" t="s">
+        <v>65</v>
+      </c>
+      <c r="J5" s="25" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" s="24">
+        <v>0</v>
+      </c>
+      <c r="B6" s="25">
+        <v>0.32490000000000002</v>
+      </c>
+      <c r="C6" s="25">
+        <v>8.2524599999999992</v>
+      </c>
+      <c r="D6" s="29">
+        <v>53.5</v>
+      </c>
+      <c r="E6" s="25">
+        <v>9.8299999999999998E-2</v>
+      </c>
+      <c r="F6" s="25">
+        <v>0.32242399999999999</v>
+      </c>
+      <c r="G6" s="25">
+        <v>245</v>
+      </c>
+      <c r="H6" s="25">
+        <v>150</v>
+      </c>
+      <c r="I6" s="25" t="s">
+        <v>67</v>
+      </c>
+      <c r="J6" s="25" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" s="24">
+        <v>1</v>
+      </c>
+      <c r="B7" s="25">
+        <v>0.2893</v>
+      </c>
+      <c r="C7" s="25">
+        <v>7.3482200000000004</v>
+      </c>
+      <c r="D7" s="29">
+        <v>42.4</v>
+      </c>
+      <c r="E7" s="25">
+        <v>0.1239</v>
+      </c>
+      <c r="F7" s="25">
+        <v>0.40639199999999998</v>
+      </c>
+      <c r="G7" s="25">
+        <v>211</v>
+      </c>
+      <c r="H7" s="25">
+        <v>119</v>
+      </c>
+      <c r="I7" s="25" t="s">
+        <v>69</v>
+      </c>
+      <c r="J7" s="25" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" s="24">
+        <v>2</v>
+      </c>
+      <c r="B8" s="25">
+        <v>0.2576</v>
+      </c>
+      <c r="C8" s="25">
+        <v>6.5430400000000004</v>
+      </c>
+      <c r="D8" s="29">
+        <v>33.6</v>
+      </c>
+      <c r="E8" s="25">
+        <v>0.15629999999999999</v>
+      </c>
+      <c r="F8" s="25">
+        <v>0.51266400000000001</v>
+      </c>
+      <c r="G8" s="25">
+        <v>181</v>
+      </c>
+      <c r="H8" s="25">
+        <v>94</v>
+      </c>
+      <c r="I8" s="25" t="s">
+        <v>71</v>
+      </c>
+      <c r="J8" s="25" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" s="24">
+        <v>3</v>
+      </c>
+      <c r="B9" s="25">
+        <v>0.22939999999999999</v>
+      </c>
+      <c r="C9" s="25">
+        <v>5.8267600000000002</v>
+      </c>
+      <c r="D9" s="29">
+        <v>26.7</v>
+      </c>
+      <c r="E9" s="25">
+        <v>0.19700000000000001</v>
+      </c>
+      <c r="F9" s="25">
+        <v>0.64615999999999996</v>
+      </c>
+      <c r="G9" s="25">
+        <v>158</v>
+      </c>
+      <c r="H9" s="25">
+        <v>75</v>
+      </c>
+      <c r="I9" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="J9" s="25" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10" s="24">
+        <v>4</v>
+      </c>
+      <c r="B10" s="25">
+        <v>0.20430000000000001</v>
+      </c>
+      <c r="C10" s="25">
+        <v>5.1892199999999997</v>
+      </c>
+      <c r="D10" s="29">
+        <v>21.1</v>
+      </c>
+      <c r="E10" s="25">
+        <v>0.2485</v>
+      </c>
+      <c r="F10" s="25">
+        <v>0.81508000000000003</v>
+      </c>
+      <c r="G10" s="25">
+        <v>135</v>
+      </c>
+      <c r="H10" s="25">
+        <v>60</v>
+      </c>
+      <c r="I10" s="25" t="s">
+        <v>75</v>
+      </c>
+      <c r="J10" s="25" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A11" s="24">
+        <v>5</v>
+      </c>
+      <c r="B11" s="25">
+        <v>0.18190000000000001</v>
+      </c>
+      <c r="C11" s="25">
+        <v>4.62026</v>
+      </c>
+      <c r="D11" s="29">
+        <v>16.8</v>
+      </c>
+      <c r="E11" s="25">
+        <v>0.31330000000000002</v>
+      </c>
+      <c r="F11" s="25">
+        <v>1.0276240000000001</v>
+      </c>
+      <c r="G11" s="25">
+        <v>118</v>
+      </c>
+      <c r="H11" s="25">
+        <v>47</v>
+      </c>
+      <c r="I11" s="25" t="s">
+        <v>77</v>
+      </c>
+      <c r="J11" s="25" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A12" s="24">
+        <v>6</v>
+      </c>
+      <c r="B12" s="25">
+        <v>0.16200000000000001</v>
+      </c>
+      <c r="C12" s="25">
+        <v>4.1147999999999998</v>
+      </c>
+      <c r="D12" s="29">
+        <v>13.3</v>
+      </c>
+      <c r="E12" s="25">
+        <v>0.39510000000000001</v>
+      </c>
+      <c r="F12" s="25">
+        <v>1.295928</v>
+      </c>
+      <c r="G12" s="25">
+        <v>101</v>
+      </c>
+      <c r="H12" s="25">
+        <v>37</v>
+      </c>
+      <c r="I12" s="25" t="s">
+        <v>79</v>
+      </c>
+      <c r="J12" s="25" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A13" s="24">
+        <v>7</v>
+      </c>
+      <c r="B13" s="25">
+        <v>0.14430000000000001</v>
+      </c>
+      <c r="C13" s="25">
+        <v>3.6652200000000001</v>
+      </c>
+      <c r="D13" s="29">
+        <v>10.6</v>
+      </c>
+      <c r="E13" s="25">
+        <v>0.49819999999999998</v>
+      </c>
+      <c r="F13" s="25">
+        <v>1.634096</v>
+      </c>
+      <c r="G13" s="25">
+        <v>89</v>
+      </c>
+      <c r="H13" s="25">
+        <v>30</v>
+      </c>
+      <c r="I13" s="25" t="s">
+        <v>81</v>
+      </c>
+      <c r="J13" s="25" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A14" s="24">
+        <v>8</v>
+      </c>
+      <c r="B14" s="25">
+        <v>0.1285</v>
+      </c>
+      <c r="C14" s="25">
+        <v>3.2639</v>
+      </c>
+      <c r="D14" s="29">
+        <v>8.3699999999999992</v>
+      </c>
+      <c r="E14" s="25">
+        <v>0.62819999999999998</v>
+      </c>
+      <c r="F14" s="25">
+        <v>2.0604960000000001</v>
+      </c>
+      <c r="G14" s="25">
+        <v>73</v>
+      </c>
+      <c r="H14" s="25">
+        <v>24</v>
+      </c>
+      <c r="I14" s="25" t="s">
+        <v>83</v>
+      </c>
+      <c r="J14" s="25" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A15" s="24">
+        <v>9</v>
+      </c>
+      <c r="B15" s="25">
+        <v>0.1144</v>
+      </c>
+      <c r="C15" s="25">
+        <v>2.9057599999999999</v>
+      </c>
+      <c r="D15" s="29">
+        <v>6.63</v>
+      </c>
+      <c r="E15" s="25">
+        <v>0.79210000000000003</v>
+      </c>
+      <c r="F15" s="25">
+        <v>2.5980880000000002</v>
+      </c>
+      <c r="G15" s="25">
+        <v>64</v>
+      </c>
+      <c r="H15" s="25">
+        <v>19</v>
+      </c>
+      <c r="I15" s="25" t="s">
+        <v>85</v>
+      </c>
+      <c r="J15" s="25" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A16" s="24">
+        <v>10</v>
+      </c>
+      <c r="B16" s="25">
+        <v>0.1019</v>
+      </c>
+      <c r="C16" s="25">
+        <v>2.58826</v>
+      </c>
+      <c r="D16" s="29">
+        <v>5.26</v>
+      </c>
+      <c r="E16" s="25">
+        <v>0.99890000000000001</v>
+      </c>
+      <c r="F16" s="25">
+        <v>3.276392</v>
+      </c>
+      <c r="G16" s="25">
+        <v>55</v>
+      </c>
+      <c r="H16" s="25">
+        <v>15</v>
+      </c>
+      <c r="I16" s="25" t="s">
+        <v>87</v>
+      </c>
+      <c r="J16" s="25" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A17" s="24">
+        <v>11</v>
+      </c>
+      <c r="B17" s="25">
+        <v>9.0700000000000003E-2</v>
+      </c>
+      <c r="C17" s="25">
+        <v>2.3037800000000002</v>
+      </c>
+      <c r="D17" s="29">
+        <v>4.17</v>
+      </c>
+      <c r="E17" s="25">
+        <v>1.26</v>
+      </c>
+      <c r="F17" s="25">
+        <v>4.1327999999999996</v>
+      </c>
+      <c r="G17" s="25">
+        <v>47</v>
+      </c>
+      <c r="H17" s="25">
+        <v>12</v>
+      </c>
+      <c r="I17" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="J17" s="25" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A18" s="24">
+        <v>12</v>
+      </c>
+      <c r="B18" s="25">
+        <v>8.0799999999999997E-2</v>
+      </c>
+      <c r="C18" s="25">
+        <v>2.0523199999999999</v>
+      </c>
+      <c r="D18" s="29">
+        <v>3.31</v>
+      </c>
+      <c r="E18" s="25">
+        <v>1.5880000000000001</v>
+      </c>
+      <c r="F18" s="25">
+        <v>5.2086399999999999</v>
+      </c>
+      <c r="G18" s="25">
+        <v>41</v>
+      </c>
+      <c r="H18" s="25">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="I18" s="25" t="s">
+        <v>91</v>
+      </c>
+      <c r="J18" s="25" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A19" s="24">
+        <v>13</v>
+      </c>
+      <c r="B19" s="25">
+        <v>7.1999999999999995E-2</v>
+      </c>
+      <c r="C19" s="25">
+        <v>1.8288</v>
+      </c>
+      <c r="D19" s="29">
+        <v>2.63</v>
+      </c>
+      <c r="E19" s="25">
+        <v>2.0030000000000001</v>
+      </c>
+      <c r="F19" s="25">
+        <v>6.5698400000000001</v>
+      </c>
+      <c r="G19" s="25">
+        <v>35</v>
+      </c>
+      <c r="H19" s="25">
+        <v>7.4</v>
+      </c>
+      <c r="I19" s="25" t="s">
+        <v>93</v>
+      </c>
+      <c r="J19" s="25" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A20" s="24">
+        <v>14</v>
+      </c>
+      <c r="B20" s="25">
+        <v>6.4100000000000004E-2</v>
+      </c>
+      <c r="C20" s="25">
+        <v>1.6281399999999999</v>
+      </c>
+      <c r="D20" s="29">
+        <v>2.08</v>
+      </c>
+      <c r="E20" s="25">
+        <v>2.5249999999999999</v>
+      </c>
+      <c r="F20" s="25">
+        <v>8.282</v>
+      </c>
+      <c r="G20" s="25">
+        <v>32</v>
+      </c>
+      <c r="H20" s="25">
+        <v>5.9</v>
+      </c>
+      <c r="I20" s="25" t="s">
+        <v>95</v>
+      </c>
+      <c r="J20" s="25" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A21" s="24">
+        <v>15</v>
+      </c>
+      <c r="B21" s="25">
+        <v>5.7099999999999998E-2</v>
+      </c>
+      <c r="C21" s="25">
+        <v>1.45034</v>
+      </c>
+      <c r="D21" s="29">
+        <v>1.65</v>
+      </c>
+      <c r="E21" s="25">
+        <v>3.1840000000000002</v>
+      </c>
+      <c r="F21" s="25">
+        <v>10.443519999999999</v>
+      </c>
+      <c r="G21" s="25">
+        <v>28</v>
+      </c>
+      <c r="H21" s="25">
+        <v>4.7</v>
+      </c>
+      <c r="I21" s="25" t="s">
+        <v>97</v>
+      </c>
+      <c r="J21" s="25" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A22" s="24">
+        <v>16</v>
+      </c>
+      <c r="B22" s="25">
+        <v>5.0799999999999998E-2</v>
+      </c>
+      <c r="C22" s="25">
+        <v>1.2903199999999999</v>
+      </c>
+      <c r="D22" s="29">
+        <v>1.31</v>
+      </c>
+      <c r="E22" s="25">
+        <v>4.016</v>
+      </c>
+      <c r="F22" s="25">
+        <v>13.17248</v>
+      </c>
+      <c r="G22" s="25">
+        <v>22</v>
+      </c>
+      <c r="H22" s="25">
+        <v>3.7</v>
+      </c>
+      <c r="I22" s="25" t="s">
+        <v>99</v>
+      </c>
+      <c r="J22" s="25" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A23" s="24">
+        <v>17</v>
+      </c>
+      <c r="B23" s="25">
+        <v>4.53E-2</v>
+      </c>
+      <c r="C23" s="25">
+        <v>1.15062</v>
+      </c>
+      <c r="D23" s="29">
+        <v>1.04</v>
+      </c>
+      <c r="E23" s="25">
+        <v>5.0640000000000001</v>
+      </c>
+      <c r="F23" s="25">
+        <v>16.609919999999999</v>
+      </c>
+      <c r="G23" s="25">
+        <v>19</v>
+      </c>
+      <c r="H23" s="25">
+        <v>2.9</v>
+      </c>
+      <c r="I23" s="25" t="s">
+        <v>101</v>
+      </c>
+      <c r="J23" s="25" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A24" s="24">
+        <v>18</v>
+      </c>
+      <c r="B24" s="25">
+        <v>4.0300000000000002E-2</v>
+      </c>
+      <c r="C24" s="25">
+        <v>1.02362</v>
+      </c>
+      <c r="D24" s="29">
+        <v>0.82299999999999995</v>
+      </c>
+      <c r="E24" s="25">
+        <v>6.3849999999999998</v>
+      </c>
+      <c r="F24" s="25">
+        <v>20.942799999999998</v>
+      </c>
+      <c r="G24" s="25">
+        <v>16</v>
+      </c>
+      <c r="H24" s="25">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="I24" s="25" t="s">
+        <v>103</v>
+      </c>
+      <c r="J24" s="25" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A25" s="24">
+        <v>19</v>
+      </c>
+      <c r="B25" s="25">
+        <v>3.5900000000000001E-2</v>
+      </c>
+      <c r="C25" s="25">
+        <v>0.91186</v>
+      </c>
+      <c r="D25" s="29">
+        <v>0.65300000000000002</v>
+      </c>
+      <c r="E25" s="25">
+        <v>8.0510000000000002</v>
+      </c>
+      <c r="F25" s="25">
+        <v>26.40728</v>
+      </c>
+      <c r="G25" s="25">
+        <v>14</v>
+      </c>
+      <c r="H25" s="25">
+        <v>1.8</v>
+      </c>
+      <c r="I25" s="25" t="s">
+        <v>105</v>
+      </c>
+      <c r="J25" s="25" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A26" s="24">
+        <v>20</v>
+      </c>
+      <c r="B26" s="25">
+        <v>3.2000000000000001E-2</v>
+      </c>
+      <c r="C26" s="25">
+        <v>0.81279999999999997</v>
+      </c>
+      <c r="D26" s="29">
+        <v>0.51900000000000002</v>
+      </c>
+      <c r="E26" s="25">
+        <v>10.15</v>
+      </c>
+      <c r="F26" s="25">
+        <v>33.292000000000002</v>
+      </c>
+      <c r="G26" s="25">
+        <v>11</v>
+      </c>
+      <c r="H26" s="25">
+        <v>1.5</v>
+      </c>
+      <c r="I26" s="25" t="s">
+        <v>107</v>
+      </c>
+      <c r="J26" s="25" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A27" s="24">
+        <v>21</v>
+      </c>
+      <c r="B27" s="25">
+        <v>2.8500000000000001E-2</v>
+      </c>
+      <c r="C27" s="25">
+        <v>0.72389999999999999</v>
+      </c>
+      <c r="D27" s="29">
+        <v>0.41199999999999998</v>
+      </c>
+      <c r="E27" s="25">
+        <v>12.8</v>
+      </c>
+      <c r="F27" s="25">
+        <v>41.984000000000002</v>
+      </c>
+      <c r="G27" s="25">
+        <v>9</v>
+      </c>
+      <c r="H27" s="25">
+        <v>1.2</v>
+      </c>
+      <c r="I27" s="25" t="s">
+        <v>109</v>
+      </c>
+      <c r="J27" s="25" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A28" s="24">
+        <v>22</v>
+      </c>
+      <c r="B28" s="25">
+        <v>2.53E-2</v>
+      </c>
+      <c r="C28" s="25">
+        <v>0.64515999999999996</v>
+      </c>
+      <c r="D28" s="29">
+        <v>0.32700000000000001</v>
+      </c>
+      <c r="E28" s="25">
+        <v>16.14</v>
+      </c>
+      <c r="F28" s="25">
+        <v>52.9392</v>
+      </c>
+      <c r="G28" s="25">
+        <v>7</v>
+      </c>
+      <c r="H28" s="25">
+        <v>0.92</v>
+      </c>
+      <c r="I28" s="25" t="s">
+        <v>111</v>
+      </c>
+      <c r="J28" s="25" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A29" s="24">
+        <v>23</v>
+      </c>
+      <c r="B29" s="25">
+        <v>2.2599999999999999E-2</v>
+      </c>
+      <c r="C29" s="25">
+        <v>0.57403999999999999</v>
+      </c>
+      <c r="D29" s="29">
+        <v>0.25900000000000001</v>
+      </c>
+      <c r="E29" s="25">
+        <v>20.36</v>
+      </c>
+      <c r="F29" s="25">
+        <v>66.780799999999999</v>
+      </c>
+      <c r="G29" s="25">
+        <v>4.7</v>
+      </c>
+      <c r="H29" s="25">
+        <v>0.72899999999999998</v>
+      </c>
+      <c r="I29" s="25" t="s">
+        <v>113</v>
+      </c>
+      <c r="J29" s="25" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A30" s="24">
+        <v>24</v>
+      </c>
+      <c r="B30" s="25">
+        <v>2.01E-2</v>
+      </c>
+      <c r="C30" s="25">
+        <v>0.51053999999999999</v>
+      </c>
+      <c r="D30" s="29">
+        <v>0.20499999999999999</v>
+      </c>
+      <c r="E30" s="25">
+        <v>25.67</v>
+      </c>
+      <c r="F30" s="25">
+        <v>84.197599999999994</v>
+      </c>
+      <c r="G30" s="25">
+        <v>3.5</v>
+      </c>
+      <c r="H30" s="25">
+        <v>0.57699999999999996</v>
+      </c>
+      <c r="I30" s="25" t="s">
+        <v>115</v>
+      </c>
+      <c r="J30" s="25" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A31" s="24">
+        <v>25</v>
+      </c>
+      <c r="B31" s="25">
+        <v>1.7899999999999999E-2</v>
+      </c>
+      <c r="C31" s="25">
+        <v>0.45466000000000001</v>
+      </c>
+      <c r="D31" s="29">
+        <v>0.16200000000000001</v>
+      </c>
+      <c r="E31" s="25">
+        <v>32.369999999999997</v>
+      </c>
+      <c r="F31" s="25">
+        <v>106.17359999999999</v>
+      </c>
+      <c r="G31" s="25">
+        <v>2.7</v>
+      </c>
+      <c r="H31" s="25">
+        <v>0.45700000000000002</v>
+      </c>
+      <c r="I31" s="25" t="s">
+        <v>117</v>
+      </c>
+      <c r="J31" s="25" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A32" s="24">
+        <v>26</v>
+      </c>
+      <c r="B32" s="25">
+        <v>1.5900000000000001E-2</v>
+      </c>
+      <c r="C32" s="25">
+        <v>0.40386</v>
+      </c>
+      <c r="D32" s="29">
+        <v>0.128</v>
+      </c>
+      <c r="E32" s="25">
+        <v>40.81</v>
+      </c>
+      <c r="F32" s="25">
+        <v>133.85679999999999</v>
+      </c>
+      <c r="G32" s="25">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="H32" s="25">
+        <v>0.36099999999999999</v>
+      </c>
+      <c r="I32" s="25" t="s">
+        <v>119</v>
+      </c>
+      <c r="J32" s="25" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A33" s="24">
+        <v>27</v>
+      </c>
+      <c r="B33" s="25">
+        <v>1.4200000000000001E-2</v>
+      </c>
+      <c r="C33" s="25">
+        <v>0.36068</v>
+      </c>
+      <c r="D33" s="29">
+        <v>0.10199999999999999</v>
+      </c>
+      <c r="E33" s="25">
+        <v>51.47</v>
+      </c>
+      <c r="F33" s="25">
+        <v>168.82159999999999</v>
+      </c>
+      <c r="G33" s="25">
+        <v>1.7</v>
+      </c>
+      <c r="H33" s="25">
+        <v>0.28799999999999998</v>
+      </c>
+      <c r="I33" s="25" t="s">
+        <v>121</v>
+      </c>
+      <c r="J33" s="25" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A34" s="24">
+        <v>28</v>
+      </c>
+      <c r="B34" s="25">
+        <v>1.26E-2</v>
+      </c>
+      <c r="C34" s="25">
+        <v>0.32003999999999999</v>
+      </c>
+      <c r="D34" s="29">
+        <v>0.08</v>
+      </c>
+      <c r="E34" s="25">
+        <v>64.900000000000006</v>
+      </c>
+      <c r="F34" s="25">
+        <v>212.87200000000001</v>
+      </c>
+      <c r="G34" s="25">
+        <v>1.4</v>
+      </c>
+      <c r="H34" s="25">
+        <v>0.22600000000000001</v>
+      </c>
+      <c r="I34" s="25" t="s">
+        <v>123</v>
+      </c>
+      <c r="J34" s="25" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A35" s="24">
+        <v>29</v>
+      </c>
+      <c r="B35" s="25">
+        <v>1.1299999999999999E-2</v>
+      </c>
+      <c r="C35" s="25">
+        <v>0.28702</v>
+      </c>
+      <c r="D35" s="29">
+        <v>6.4699999999999994E-2</v>
+      </c>
+      <c r="E35" s="25">
+        <v>81.83</v>
+      </c>
+      <c r="F35" s="25">
+        <v>268.4024</v>
+      </c>
+      <c r="G35" s="25">
+        <v>1.2</v>
+      </c>
+      <c r="H35" s="25">
+        <v>0.182</v>
+      </c>
+      <c r="I35" s="25" t="s">
+        <v>125</v>
+      </c>
+      <c r="J35" s="25" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A36" s="24">
+        <v>30</v>
+      </c>
+      <c r="B36" s="25">
+        <v>0.01</v>
+      </c>
+      <c r="C36" s="25">
+        <v>0.254</v>
+      </c>
+      <c r="D36" s="29">
+        <v>5.0700000000000002E-2</v>
+      </c>
+      <c r="E36" s="25">
+        <v>103.2</v>
+      </c>
+      <c r="F36" s="25">
+        <v>338.49599999999998</v>
+      </c>
+      <c r="G36" s="25">
+        <v>0.86</v>
+      </c>
+      <c r="H36" s="25">
+        <v>0.14199999999999999</v>
+      </c>
+      <c r="I36" s="25" t="s">
+        <v>127</v>
+      </c>
+      <c r="J36" s="25" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A37" s="24">
+        <v>31</v>
+      </c>
+      <c r="B37" s="25">
+        <v>8.8999999999999999E-3</v>
+      </c>
+      <c r="C37" s="25">
+        <v>0.22606000000000001</v>
+      </c>
+      <c r="D37" s="29">
+        <v>4.0099999999999997E-2</v>
+      </c>
+      <c r="E37" s="25">
+        <v>130.1</v>
+      </c>
+      <c r="F37" s="25">
+        <v>426.72800000000001</v>
+      </c>
+      <c r="G37" s="25">
+        <v>0.7</v>
+      </c>
+      <c r="H37" s="25">
+        <v>0.113</v>
+      </c>
+      <c r="I37" s="25" t="s">
+        <v>129</v>
+      </c>
+      <c r="J37" s="25" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A38" s="24">
+        <v>32</v>
+      </c>
+      <c r="B38" s="25">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="C38" s="25">
+        <v>0.20319999999999999</v>
+      </c>
+      <c r="D38" s="29">
+        <v>3.2399999999999998E-2</v>
+      </c>
+      <c r="E38" s="25">
+        <v>164.1</v>
+      </c>
+      <c r="F38" s="25">
+        <v>538.24800000000005</v>
+      </c>
+      <c r="G38" s="25">
+        <v>0.53</v>
+      </c>
+      <c r="H38" s="25">
+        <v>9.0999999999999998E-2</v>
+      </c>
+      <c r="I38" s="25" t="s">
+        <v>131</v>
+      </c>
+      <c r="J38" s="25" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A39" s="24" t="s">
+        <v>133</v>
+      </c>
+      <c r="B39" s="25">
+        <v>7.8700000000000003E-3</v>
+      </c>
+      <c r="C39" s="25">
+        <v>0.2</v>
+      </c>
+      <c r="D39" s="29">
+        <v>3.1399999999999997E-2</v>
+      </c>
+      <c r="E39" s="25">
+        <v>169.39</v>
+      </c>
+      <c r="F39" s="25">
+        <v>555.61</v>
+      </c>
+      <c r="G39" s="25">
+        <v>0.51</v>
+      </c>
+      <c r="H39" s="25">
+        <v>8.7999999999999995E-2</v>
+      </c>
+      <c r="I39" s="25" t="s">
+        <v>134</v>
+      </c>
+      <c r="J39" s="25"/>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="J1:J2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EE355BF-C773-4D1D-B00A-4E91F8B61265}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -1534,7 +3320,7 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C208A52-CC99-4AA1-B3E0-B21E40CC73B4}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{040A89E2-B5A4-4047-A575-DB67B7BEB714}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
     <ds:schemaRef ds:uri="http://www.boldonjames.com/2008/01/sie/internal/label"/>

</xml_diff>

<commit_message>
Cable resistances were added
</commit_message>
<xml_diff>
--- a/Magnetic Design/Transformer_Design_Excel.xlsx
+++ b/Magnetic Design/Transformer_Design_Excel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahmetcan.akuz\Documents\GitHub\Optimus-Primary-Winding\Magnetic Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B25FB1C-C476-4F24-A04E-0F2B2154EBE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99F8C8B1-2E0C-4160-B972-16F1351E10A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="11364" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Transformer_Design" sheetId="1" r:id="rId1"/>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="149">
   <si>
     <t>Voltage Pri Min</t>
   </si>
@@ -501,6 +501,24 @@
   </si>
   <si>
     <t xml:space="preserve"> Selected Core Name:</t>
+  </si>
+  <si>
+    <t>MLT</t>
+  </si>
+  <si>
+    <t>R_pri</t>
+  </si>
+  <si>
+    <t>R_sec</t>
+  </si>
+  <si>
+    <t>resis_pri</t>
+  </si>
+  <si>
+    <t>resis_sec</t>
+  </si>
+  <si>
+    <t>mOhm</t>
   </si>
 </sst>
 </file>
@@ -797,7 +815,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -821,6 +839,12 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -854,24 +878,19 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Check Cell" xfId="1" builtinId="23"/>
@@ -1548,10 +1567,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P37"/>
+  <dimension ref="A1:P40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="K27" sqref="K27"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="M28" sqref="M28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1566,11 +1585,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="18"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="20"/>
     </row>
     <row r="2" spans="1:16" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
@@ -1661,12 +1680,12 @@
       <c r="F9" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="G9" s="25" t="s">
+      <c r="G9" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="H9" s="25"/>
-      <c r="I9" s="25"/>
-      <c r="J9" s="25"/>
+      <c r="H9" s="27"/>
+      <c r="I9" s="27"/>
+      <c r="J9" s="27"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10" s="10" t="s">
@@ -1678,11 +1697,11 @@
       <c r="C10" s="1"/>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A11" s="19" t="s">
+      <c r="A11" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="20"/>
-      <c r="C11" s="21"/>
+      <c r="B11" s="22"/>
+      <c r="C11" s="23"/>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
@@ -1748,11 +1767,11 @@
       <c r="C16" s="1"/>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A17" s="22" t="s">
+      <c r="A17" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="23"/>
-      <c r="C17" s="24"/>
+      <c r="B17" s="25"/>
+      <c r="C17" s="26"/>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
@@ -1806,14 +1825,14 @@
       <c r="C21" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D21" s="30" t="s">
+      <c r="D21" s="28" t="s">
         <v>142</v>
       </c>
-      <c r="E21" s="30"/>
-      <c r="F21" s="31" t="s">
+      <c r="E21" s="28"/>
+      <c r="F21" s="29" t="s">
         <v>141</v>
       </c>
-      <c r="G21" s="31"/>
+      <c r="G21" s="29"/>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
@@ -1884,8 +1903,8 @@
         <v>16</v>
       </c>
       <c r="C27" s="7"/>
-      <c r="F27" s="15"/>
-      <c r="G27" s="15"/>
+      <c r="F27" s="17"/>
+      <c r="G27" s="17"/>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
@@ -1948,11 +1967,11 @@
       <c r="D32" s="8"/>
       <c r="F32" s="8"/>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A33" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="B33" s="1">
+      <c r="B33" s="7">
         <f>B29/B31</f>
         <v>0.38423368514245931</v>
       </c>
@@ -1960,7 +1979,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>135</v>
       </c>
@@ -1994,8 +2013,15 @@
         <f ca="1">ROUNDUP(B32/D34,0)</f>
         <v>8</v>
       </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K34" s="32" t="s">
+        <v>146</v>
+      </c>
+      <c r="L34" s="1" cm="1">
+        <f t="array" aca="1" ref="L34" ca="1">INDIRECT("AWG!F" &amp; B34+6)</f>
+        <v>84.197599999999994</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>137</v>
       </c>
@@ -2029,12 +2055,19 @@
         <f ca="1">ROUNDUP(B33/D35,0)</f>
         <v>2</v>
       </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K35" s="32" t="s">
+        <v>147</v>
+      </c>
+      <c r="L35" s="1" cm="1">
+        <f t="array" aca="1" ref="L35" ca="1">INDIRECT("AWG!F" &amp; B35+6)</f>
+        <v>84.197599999999994</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A36" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="B36" s="1">
+      <c r="B36" s="14">
         <f ca="1">D34*J34*B25+D35*J35*B27</f>
         <v>13.12</v>
       </c>
@@ -2042,15 +2075,58 @@
         <v>23</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A37" s="4" t="s">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A37" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="B37" s="1">
+      <c r="B37" s="7">
         <f ca="1">B36/B20</f>
         <v>3.5080213903743315E-2</v>
       </c>
-      <c r="C37" s="1"/>
+      <c r="C37" s="7"/>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A38" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="B38" s="1">
+        <f>2*3.14*(30.9-12.2)/2</f>
+        <v>58.718000000000004</v>
+      </c>
+      <c r="C38" s="1"/>
+      <c r="D38" s="1"/>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A39" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="B39" s="1">
+        <f ca="1">(B25*B38*L34)/(J34*10^6)</f>
+        <v>2.4719573384000002E-3</v>
+      </c>
+      <c r="C39" s="1">
+        <f ca="1">1000*B39</f>
+        <v>2.4719573384000002</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A40" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="B40" s="1">
+        <f ca="1">(B27*B38*L35)/(J35*10^6)</f>
+        <v>3.9551317414400003E-2</v>
+      </c>
+      <c r="C40" s="1">
+        <f ca="1">1000*B40</f>
+        <v>39.551317414400003</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>148</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -2071,7 +2147,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B96DE545-7F3F-4161-810A-0A86D0D5D381}">
   <dimension ref="A1:J39"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O38" sqref="O38"/>
     </sheetView>
   </sheetViews>
@@ -2082,7 +2158,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="30" t="s">
         <v>48</v>
       </c>
       <c r="B1" s="11" t="s">
@@ -2091,16 +2167,16 @@
       <c r="C1" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="D1" s="26" t="s">
+      <c r="D1" s="30" t="s">
         <v>52</v>
       </c>
-      <c r="E1" s="26" t="s">
+      <c r="E1" s="30" t="s">
         <v>53</v>
       </c>
-      <c r="F1" s="26" t="s">
+      <c r="F1" s="30" t="s">
         <v>54</v>
       </c>
-      <c r="G1" s="26" t="s">
+      <c r="G1" s="30" t="s">
         <v>55</v>
       </c>
       <c r="H1" s="11" t="s">
@@ -2109,41 +2185,41 @@
       <c r="I1" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="J1" s="26" t="s">
+      <c r="J1" s="30" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="35.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="27"/>
+      <c r="A2" s="31"/>
       <c r="B2" s="12" t="s">
         <v>50</v>
       </c>
       <c r="C2" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="31"/>
       <c r="H2" s="12" t="s">
         <v>57</v>
       </c>
       <c r="I2" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="J2" s="27"/>
+      <c r="J2" s="31"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="29">
+      <c r="A3" s="16">
         <v>0</v>
       </c>
       <c r="B3" s="13">
         <v>0.46</v>
       </c>
-      <c r="C3" s="28">
+      <c r="C3" s="15">
         <v>11.683999999999999</v>
       </c>
-      <c r="D3" s="28">
+      <c r="D3" s="15">
         <v>107</v>
       </c>
       <c r="E3" s="13">
@@ -2166,16 +2242,16 @@
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" s="29">
+      <c r="A4" s="16">
         <v>0</v>
       </c>
       <c r="B4" s="13">
         <v>0.40960000000000002</v>
       </c>
-      <c r="C4" s="28">
+      <c r="C4" s="15">
         <v>10.403840000000001</v>
       </c>
-      <c r="D4" s="28">
+      <c r="D4" s="15">
         <v>84.9</v>
       </c>
       <c r="E4" s="13">
@@ -2198,16 +2274,16 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" s="29">
+      <c r="A5" s="16">
         <v>0</v>
       </c>
       <c r="B5" s="13">
         <v>0.36480000000000001</v>
       </c>
-      <c r="C5" s="28">
+      <c r="C5" s="15">
         <v>9.2659199999999995</v>
       </c>
-      <c r="D5" s="28">
+      <c r="D5" s="15">
         <v>67.400000000000006</v>
       </c>
       <c r="E5" s="13">
@@ -2230,16 +2306,16 @@
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" s="29">
+      <c r="A6" s="16">
         <v>0</v>
       </c>
       <c r="B6" s="13">
         <v>0.32490000000000002</v>
       </c>
-      <c r="C6" s="28">
+      <c r="C6" s="15">
         <v>8.2524599999999992</v>
       </c>
-      <c r="D6" s="28">
+      <c r="D6" s="15">
         <v>53.5</v>
       </c>
       <c r="E6" s="13">
@@ -2262,16 +2338,16 @@
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A7" s="29">
+      <c r="A7" s="16">
         <v>1</v>
       </c>
       <c r="B7" s="13">
         <v>0.2893</v>
       </c>
-      <c r="C7" s="28">
+      <c r="C7" s="15">
         <v>7.3482200000000004</v>
       </c>
-      <c r="D7" s="28">
+      <c r="D7" s="15">
         <v>42.4</v>
       </c>
       <c r="E7" s="13">
@@ -2294,16 +2370,16 @@
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8" s="29">
+      <c r="A8" s="16">
         <v>2</v>
       </c>
       <c r="B8" s="13">
         <v>0.2576</v>
       </c>
-      <c r="C8" s="28">
+      <c r="C8" s="15">
         <v>6.5430400000000004</v>
       </c>
-      <c r="D8" s="28">
+      <c r="D8" s="15">
         <v>33.6</v>
       </c>
       <c r="E8" s="13">
@@ -2326,16 +2402,16 @@
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A9" s="29">
+      <c r="A9" s="16">
         <v>3</v>
       </c>
       <c r="B9" s="13">
         <v>0.22939999999999999</v>
       </c>
-      <c r="C9" s="28">
+      <c r="C9" s="15">
         <v>5.8267600000000002</v>
       </c>
-      <c r="D9" s="28">
+      <c r="D9" s="15">
         <v>26.7</v>
       </c>
       <c r="E9" s="13">
@@ -2358,16 +2434,16 @@
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A10" s="29">
+      <c r="A10" s="16">
         <v>4</v>
       </c>
       <c r="B10" s="13">
         <v>0.20430000000000001</v>
       </c>
-      <c r="C10" s="28">
+      <c r="C10" s="15">
         <v>5.1892199999999997</v>
       </c>
-      <c r="D10" s="28">
+      <c r="D10" s="15">
         <v>21.1</v>
       </c>
       <c r="E10" s="13">
@@ -2390,16 +2466,16 @@
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A11" s="29">
+      <c r="A11" s="16">
         <v>5</v>
       </c>
       <c r="B11" s="13">
         <v>0.18190000000000001</v>
       </c>
-      <c r="C11" s="28">
+      <c r="C11" s="15">
         <v>4.62026</v>
       </c>
-      <c r="D11" s="28">
+      <c r="D11" s="15">
         <v>16.8</v>
       </c>
       <c r="E11" s="13">
@@ -2422,16 +2498,16 @@
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A12" s="29">
+      <c r="A12" s="16">
         <v>6</v>
       </c>
       <c r="B12" s="13">
         <v>0.16200000000000001</v>
       </c>
-      <c r="C12" s="28">
+      <c r="C12" s="15">
         <v>4.1147999999999998</v>
       </c>
-      <c r="D12" s="28">
+      <c r="D12" s="15">
         <v>13.3</v>
       </c>
       <c r="E12" s="13">
@@ -2454,16 +2530,16 @@
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A13" s="29">
+      <c r="A13" s="16">
         <v>7</v>
       </c>
       <c r="B13" s="13">
         <v>0.14430000000000001</v>
       </c>
-      <c r="C13" s="28">
+      <c r="C13" s="15">
         <v>3.6652200000000001</v>
       </c>
-      <c r="D13" s="28">
+      <c r="D13" s="15">
         <v>10.6</v>
       </c>
       <c r="E13" s="13">
@@ -2486,16 +2562,16 @@
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A14" s="29">
+      <c r="A14" s="16">
         <v>8</v>
       </c>
       <c r="B14" s="13">
         <v>0.1285</v>
       </c>
-      <c r="C14" s="28">
+      <c r="C14" s="15">
         <v>3.2639</v>
       </c>
-      <c r="D14" s="28">
+      <c r="D14" s="15">
         <v>8.3699999999999992</v>
       </c>
       <c r="E14" s="13">
@@ -2518,16 +2594,16 @@
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A15" s="29">
+      <c r="A15" s="16">
         <v>9</v>
       </c>
       <c r="B15" s="13">
         <v>0.1144</v>
       </c>
-      <c r="C15" s="28">
+      <c r="C15" s="15">
         <v>2.9057599999999999</v>
       </c>
-      <c r="D15" s="28">
+      <c r="D15" s="15">
         <v>6.63</v>
       </c>
       <c r="E15" s="13">
@@ -2550,16 +2626,16 @@
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A16" s="29">
+      <c r="A16" s="16">
         <v>10</v>
       </c>
       <c r="B16" s="13">
         <v>0.1019</v>
       </c>
-      <c r="C16" s="28">
+      <c r="C16" s="15">
         <v>2.58826</v>
       </c>
-      <c r="D16" s="28">
+      <c r="D16" s="15">
         <v>5.26</v>
       </c>
       <c r="E16" s="13">
@@ -2582,16 +2658,16 @@
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A17" s="29">
+      <c r="A17" s="16">
         <v>11</v>
       </c>
       <c r="B17" s="13">
         <v>9.0700000000000003E-2</v>
       </c>
-      <c r="C17" s="28">
+      <c r="C17" s="15">
         <v>2.3037800000000002</v>
       </c>
-      <c r="D17" s="28">
+      <c r="D17" s="15">
         <v>4.17</v>
       </c>
       <c r="E17" s="13">
@@ -2614,16 +2690,16 @@
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A18" s="29">
+      <c r="A18" s="16">
         <v>12</v>
       </c>
       <c r="B18" s="13">
         <v>8.0799999999999997E-2</v>
       </c>
-      <c r="C18" s="28">
+      <c r="C18" s="15">
         <v>2.0523199999999999</v>
       </c>
-      <c r="D18" s="28">
+      <c r="D18" s="15">
         <v>3.31</v>
       </c>
       <c r="E18" s="13">
@@ -2646,16 +2722,16 @@
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A19" s="29">
+      <c r="A19" s="16">
         <v>13</v>
       </c>
       <c r="B19" s="13">
         <v>7.1999999999999995E-2</v>
       </c>
-      <c r="C19" s="28">
+      <c r="C19" s="15">
         <v>1.8288</v>
       </c>
-      <c r="D19" s="28">
+      <c r="D19" s="15">
         <v>2.63</v>
       </c>
       <c r="E19" s="13">
@@ -2678,16 +2754,16 @@
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A20" s="29">
+      <c r="A20" s="16">
         <v>14</v>
       </c>
       <c r="B20" s="13">
         <v>6.4100000000000004E-2</v>
       </c>
-      <c r="C20" s="28">
+      <c r="C20" s="15">
         <v>1.6281399999999999</v>
       </c>
-      <c r="D20" s="28">
+      <c r="D20" s="15">
         <v>2.08</v>
       </c>
       <c r="E20" s="13">
@@ -2710,16 +2786,16 @@
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A21" s="29">
+      <c r="A21" s="16">
         <v>15</v>
       </c>
       <c r="B21" s="13">
         <v>5.7099999999999998E-2</v>
       </c>
-      <c r="C21" s="28">
+      <c r="C21" s="15">
         <v>1.45034</v>
       </c>
-      <c r="D21" s="28">
+      <c r="D21" s="15">
         <v>1.65</v>
       </c>
       <c r="E21" s="13">
@@ -2742,16 +2818,16 @@
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A22" s="29">
+      <c r="A22" s="16">
         <v>16</v>
       </c>
       <c r="B22" s="13">
         <v>5.0799999999999998E-2</v>
       </c>
-      <c r="C22" s="28">
+      <c r="C22" s="15">
         <v>1.2903199999999999</v>
       </c>
-      <c r="D22" s="28">
+      <c r="D22" s="15">
         <v>1.31</v>
       </c>
       <c r="E22" s="13">
@@ -2774,16 +2850,16 @@
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A23" s="29">
+      <c r="A23" s="16">
         <v>17</v>
       </c>
       <c r="B23" s="13">
         <v>4.53E-2</v>
       </c>
-      <c r="C23" s="28">
+      <c r="C23" s="15">
         <v>1.15062</v>
       </c>
-      <c r="D23" s="28">
+      <c r="D23" s="15">
         <v>1.04</v>
       </c>
       <c r="E23" s="13">
@@ -2806,16 +2882,16 @@
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A24" s="29">
+      <c r="A24" s="16">
         <v>18</v>
       </c>
       <c r="B24" s="13">
         <v>4.0300000000000002E-2</v>
       </c>
-      <c r="C24" s="28">
+      <c r="C24" s="15">
         <v>1.02362</v>
       </c>
-      <c r="D24" s="28">
+      <c r="D24" s="15">
         <v>0.82299999999999995</v>
       </c>
       <c r="E24" s="13">
@@ -2838,16 +2914,16 @@
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A25" s="29">
+      <c r="A25" s="16">
         <v>19</v>
       </c>
       <c r="B25" s="13">
         <v>3.5900000000000001E-2</v>
       </c>
-      <c r="C25" s="28">
+      <c r="C25" s="15">
         <v>0.91186</v>
       </c>
-      <c r="D25" s="28">
+      <c r="D25" s="15">
         <v>0.65300000000000002</v>
       </c>
       <c r="E25" s="13">
@@ -2870,16 +2946,16 @@
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A26" s="29">
+      <c r="A26" s="16">
         <v>20</v>
       </c>
       <c r="B26" s="13">
         <v>3.2000000000000001E-2</v>
       </c>
-      <c r="C26" s="28">
+      <c r="C26" s="15">
         <v>0.81279999999999997</v>
       </c>
-      <c r="D26" s="28">
+      <c r="D26" s="15">
         <v>0.51900000000000002</v>
       </c>
       <c r="E26" s="13">
@@ -2902,16 +2978,16 @@
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A27" s="29">
+      <c r="A27" s="16">
         <v>21</v>
       </c>
       <c r="B27" s="13">
         <v>2.8500000000000001E-2</v>
       </c>
-      <c r="C27" s="28">
+      <c r="C27" s="15">
         <v>0.72389999999999999</v>
       </c>
-      <c r="D27" s="28">
+      <c r="D27" s="15">
         <v>0.41199999999999998</v>
       </c>
       <c r="E27" s="13">
@@ -2934,16 +3010,16 @@
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A28" s="29">
+      <c r="A28" s="16">
         <v>22</v>
       </c>
       <c r="B28" s="13">
         <v>2.53E-2</v>
       </c>
-      <c r="C28" s="28">
+      <c r="C28" s="15">
         <v>0.64515999999999996</v>
       </c>
-      <c r="D28" s="28">
+      <c r="D28" s="15">
         <v>0.32700000000000001</v>
       </c>
       <c r="E28" s="13">
@@ -2966,16 +3042,16 @@
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A29" s="29">
+      <c r="A29" s="16">
         <v>23</v>
       </c>
       <c r="B29" s="13">
         <v>2.2599999999999999E-2</v>
       </c>
-      <c r="C29" s="28">
+      <c r="C29" s="15">
         <v>0.57403999999999999</v>
       </c>
-      <c r="D29" s="28">
+      <c r="D29" s="15">
         <v>0.25900000000000001</v>
       </c>
       <c r="E29" s="13">
@@ -2998,16 +3074,16 @@
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A30" s="29">
+      <c r="A30" s="16">
         <v>24</v>
       </c>
       <c r="B30" s="13">
         <v>2.01E-2</v>
       </c>
-      <c r="C30" s="28">
+      <c r="C30" s="15">
         <v>0.51053999999999999</v>
       </c>
-      <c r="D30" s="28">
+      <c r="D30" s="15">
         <v>0.20499999999999999</v>
       </c>
       <c r="E30" s="13">
@@ -3030,16 +3106,16 @@
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A31" s="29">
+      <c r="A31" s="16">
         <v>25</v>
       </c>
       <c r="B31" s="13">
         <v>1.7899999999999999E-2</v>
       </c>
-      <c r="C31" s="28">
+      <c r="C31" s="15">
         <v>0.45466000000000001</v>
       </c>
-      <c r="D31" s="28">
+      <c r="D31" s="15">
         <v>0.16200000000000001</v>
       </c>
       <c r="E31" s="13">
@@ -3062,16 +3138,16 @@
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A32" s="29">
+      <c r="A32" s="16">
         <v>26</v>
       </c>
       <c r="B32" s="13">
         <v>1.5900000000000001E-2</v>
       </c>
-      <c r="C32" s="28">
+      <c r="C32" s="15">
         <v>0.40386</v>
       </c>
-      <c r="D32" s="28">
+      <c r="D32" s="15">
         <v>0.128</v>
       </c>
       <c r="E32" s="13">
@@ -3094,16 +3170,16 @@
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A33" s="29">
+      <c r="A33" s="16">
         <v>27</v>
       </c>
       <c r="B33" s="13">
         <v>1.4200000000000001E-2</v>
       </c>
-      <c r="C33" s="28">
+      <c r="C33" s="15">
         <v>0.36068</v>
       </c>
-      <c r="D33" s="28">
+      <c r="D33" s="15">
         <v>0.10199999999999999</v>
       </c>
       <c r="E33" s="13">
@@ -3126,16 +3202,16 @@
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A34" s="29">
+      <c r="A34" s="16">
         <v>28</v>
       </c>
       <c r="B34" s="13">
         <v>1.26E-2</v>
       </c>
-      <c r="C34" s="28">
+      <c r="C34" s="15">
         <v>0.32003999999999999</v>
       </c>
-      <c r="D34" s="28">
+      <c r="D34" s="15">
         <v>0.08</v>
       </c>
       <c r="E34" s="13">
@@ -3158,16 +3234,16 @@
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A35" s="29">
+      <c r="A35" s="16">
         <v>29</v>
       </c>
       <c r="B35" s="13">
         <v>1.1299999999999999E-2</v>
       </c>
-      <c r="C35" s="28">
+      <c r="C35" s="15">
         <v>0.28702</v>
       </c>
-      <c r="D35" s="28">
+      <c r="D35" s="15">
         <v>6.4699999999999994E-2</v>
       </c>
       <c r="E35" s="13">
@@ -3190,16 +3266,16 @@
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A36" s="29">
+      <c r="A36" s="16">
         <v>30</v>
       </c>
       <c r="B36" s="13">
         <v>0.01</v>
       </c>
-      <c r="C36" s="28">
+      <c r="C36" s="15">
         <v>0.254</v>
       </c>
-      <c r="D36" s="28">
+      <c r="D36" s="15">
         <v>5.0700000000000002E-2</v>
       </c>
       <c r="E36" s="13">
@@ -3222,16 +3298,16 @@
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A37" s="29">
+      <c r="A37" s="16">
         <v>31</v>
       </c>
       <c r="B37" s="13">
         <v>8.8999999999999999E-3</v>
       </c>
-      <c r="C37" s="28">
+      <c r="C37" s="15">
         <v>0.22606000000000001</v>
       </c>
-      <c r="D37" s="28">
+      <c r="D37" s="15">
         <v>4.0099999999999997E-2</v>
       </c>
       <c r="E37" s="13">
@@ -3254,16 +3330,16 @@
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A38" s="29">
+      <c r="A38" s="16">
         <v>32</v>
       </c>
       <c r="B38" s="13">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="C38" s="28">
+      <c r="C38" s="15">
         <v>0.20319999999999999</v>
       </c>
-      <c r="D38" s="28">
+      <c r="D38" s="15">
         <v>3.2399999999999998E-2</v>
       </c>
       <c r="E38" s="13">
@@ -3286,16 +3362,16 @@
       </c>
     </row>
     <row r="39" spans="1:10" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A39" s="29" t="s">
+      <c r="A39" s="16" t="s">
         <v>133</v>
       </c>
       <c r="B39" s="13">
         <v>7.8700000000000003E-3</v>
       </c>
-      <c r="C39" s="28">
+      <c r="C39" s="15">
         <v>0.2</v>
       </c>
-      <c r="D39" s="28">
+      <c r="D39" s="15">
         <v>3.1399999999999997E-2</v>
       </c>
       <c r="E39" s="13">
@@ -3349,7 +3425,7 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{23CB67D2-12A4-42A0-8780-C1787795E96F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{27D7E5FF-15EE-4F2A-872A-6A49A9D7F096}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
     <ds:schemaRef ds:uri="http://www.boldonjames.com/2008/01/sie/internal/label"/>

</xml_diff>

<commit_message>
Magnetic Design Parameters were finalized
</commit_message>
<xml_diff>
--- a/Magnetic Design/Transformer_Design_Excel.xlsx
+++ b/Magnetic Design/Transformer_Design_Excel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahmetcan.akuz\Documents\GitHub\Optimus-Primary-Winding\Magnetic Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99F8C8B1-2E0C-4160-B972-16F1351E10A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4064970-67D8-43DD-841F-F16BE05031D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="13776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Transformer_Design" sheetId="1" r:id="rId1"/>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="150">
   <si>
     <t>Voltage Pri Min</t>
   </si>
@@ -174,12 +174,6 @@
   </si>
   <si>
     <t>nH/turns^2</t>
-  </si>
-  <si>
-    <t>Gap length, G</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mm </t>
   </si>
   <si>
     <t>Current Desity, J</t>
@@ -519,6 +513,15 @@
   </si>
   <si>
     <t>mOhm</t>
+  </si>
+  <si>
+    <t>Le</t>
+  </si>
+  <si>
+    <t>Gap length, l_g</t>
+  </si>
+  <si>
+    <t>Permiability, u (ungapped)</t>
   </si>
 </sst>
 </file>
@@ -815,7 +818,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -890,7 +893,6 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Check Cell" xfId="1" builtinId="23"/>
@@ -1214,6 +1216,50 @@
         <a:xfrm>
           <a:off x="7627620" y="2918460"/>
           <a:ext cx="1813559" cy="647700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>7620</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>160020</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>533565</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>30548</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{403AB5A5-117A-7FCF-1E74-12689AE5D843}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4290060" y="6979920"/>
+          <a:ext cx="1905165" cy="784928"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1567,10 +1613,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P40"/>
+  <dimension ref="A1:P42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="M28" sqref="M28"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1689,7 +1735,7 @@
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10" s="10" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B10" s="1">
         <v>0.4</v>
@@ -1806,7 +1852,7 @@
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B20" s="5">
         <v>374</v>
@@ -1826,11 +1872,11 @@
         <v>37</v>
       </c>
       <c r="D21" s="28" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E21" s="28"/>
       <c r="F21" s="29" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="G21" s="29"/>
     </row>
@@ -1917,6 +1963,10 @@
       <c r="C28" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="I28">
+        <f>1000*D22/16</f>
+        <v>830.07812500000011</v>
+      </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
@@ -1931,52 +1981,82 @@
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A30" s="4" t="s">
+      <c r="A30" s="2" t="s">
         <v>38</v>
       </c>
       <c r="B30" s="1">
-        <f>40*3.14*B19*(((B23^2)/(1000*B23))+(1/B21))</f>
-        <v>110.29451282051284</v>
+        <v>5</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A31" s="2" t="s">
-        <v>40</v>
+      <c r="A31" s="4" t="s">
+        <v>42</v>
       </c>
       <c r="B31" s="1">
-        <v>5</v>
+        <f>B15/B30</f>
+        <v>1.5369347405698373</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>41</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="D31" s="8"/>
+      <c r="F31" s="8"/>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A32" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="B32" s="1">
-        <f>B15/B31</f>
-        <v>1.5369347405698373</v>
-      </c>
-      <c r="C32" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B32" s="7">
+        <f>B29/B30</f>
+        <v>0.38423368514245931</v>
+      </c>
+      <c r="C32" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="D32" s="8"/>
-      <c r="F32" s="8"/>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A33" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="B33" s="7">
-        <f>B29/B31</f>
-        <v>0.38423368514245931</v>
-      </c>
-      <c r="C33" s="7" t="s">
+      <c r="A33" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="B33" s="1">
+        <v>24</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="D33" s="1" cm="1">
+        <f t="array" aca="1" ref="D33" ca="1">INDIRECT("AWG!D" &amp; B33+6)</f>
+        <v>0.20499999999999999</v>
+      </c>
+      <c r="E33" s="1" t="s">
         <v>23</v>
+      </c>
+      <c r="F33" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="G33" s="1" cm="1">
+        <f t="array" aca="1" ref="G33" ca="1">INDIRECT("AWG!C" &amp; B33+6)</f>
+        <v>0.51053999999999999</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="I33" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="J33" s="1">
+        <f ca="1">ROUNDUP(B31/D33,0)</f>
+        <v>8</v>
+      </c>
+      <c r="K33" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="L33" s="1" cm="1">
+        <f t="array" aca="1" ref="L33" ca="1">INDIRECT("AWG!F" &amp; B33+6)</f>
+        <v>84.197599999999994</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.3">
@@ -1987,7 +2067,7 @@
         <v>24</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D34" s="1" cm="1">
         <f t="array" aca="1" ref="D34" ca="1">INDIRECT("AWG!D" &amp; B34+6)</f>
@@ -1997,24 +2077,24 @@
         <v>23</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="G34" s="1" cm="1">
         <f t="array" aca="1" ref="G34" ca="1">INDIRECT("AWG!C" &amp; B34+6)</f>
         <v>0.51053999999999999</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="I34" s="4" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="J34" s="1">
         <f ca="1">ROUNDUP(B32/D34,0)</f>
-        <v>8</v>
-      </c>
-      <c r="K34" s="32" t="s">
-        <v>146</v>
+        <v>2</v>
+      </c>
+      <c r="K34" s="1" t="s">
+        <v>145</v>
       </c>
       <c r="L34" s="1" cm="1">
         <f t="array" aca="1" ref="L34" ca="1">INDIRECT("AWG!F" &amp; B34+6)</f>
@@ -2022,86 +2102,56 @@
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A35" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="B35" s="1">
-        <v>24</v>
-      </c>
-      <c r="C35" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="D35" s="1" cm="1">
-        <f t="array" aca="1" ref="D35" ca="1">INDIRECT("AWG!D" &amp; B35+6)</f>
-        <v>0.20499999999999999</v>
-      </c>
-      <c r="E35" s="1" t="s">
+      <c r="A35" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B35" s="14">
+        <f ca="1">D33*J33*B25+D34*J34*B27</f>
+        <v>13.12</v>
+      </c>
+      <c r="C35" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="F35" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="G35" s="1" cm="1">
-        <f t="array" aca="1" ref="G35" ca="1">INDIRECT("AWG!C" &amp; B35+6)</f>
-        <v>0.51053999999999999</v>
-      </c>
-      <c r="H35" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="I35" s="4" t="s">
-        <v>139</v>
-      </c>
-      <c r="J35" s="1">
-        <f ca="1">ROUNDUP(B33/D35,0)</f>
-        <v>2</v>
-      </c>
-      <c r="K35" s="32" t="s">
-        <v>147</v>
-      </c>
-      <c r="L35" s="1" cm="1">
-        <f t="array" aca="1" ref="L35" ca="1">INDIRECT("AWG!F" &amp; B35+6)</f>
-        <v>84.197599999999994</v>
-      </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A36" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="B36" s="14">
-        <f ca="1">D34*J34*B25+D35*J35*B27</f>
-        <v>13.12</v>
-      </c>
-      <c r="C36" s="14" t="s">
-        <v>23</v>
-      </c>
+      <c r="A36" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B36" s="7">
+        <f ca="1">B35/B20</f>
+        <v>3.5080213903743315E-2</v>
+      </c>
+      <c r="C36" s="7"/>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A37" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="B37" s="7">
-        <f ca="1">B36/B20</f>
-        <v>3.5080213903743315E-2</v>
-      </c>
-      <c r="C37" s="7"/>
+      <c r="A37" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="B37" s="1">
+        <f>2*3.14*(30.9-12.2)/2</f>
+        <v>58.718000000000004</v>
+      </c>
+      <c r="C37" s="1"/>
+      <c r="D37" s="1"/>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="B38" s="1">
-        <f>2*3.14*(30.9-12.2)/2</f>
-        <v>58.718000000000004</v>
-      </c>
-      <c r="C38" s="1"/>
+        <v>97</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>138</v>
+      </c>
       <c r="D38" s="1"/>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A39" s="4" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B39" s="1">
-        <f ca="1">(B25*B38*L34)/(J34*10^6)</f>
+        <f ca="1">(B25*B37*L33)/(J33*10^6)</f>
         <v>2.4719573384000002E-3</v>
       </c>
       <c r="C39" s="1">
@@ -2109,15 +2159,15 @@
         <v>2.4719573384000002</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A40" s="4" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B40" s="1">
-        <f ca="1">(B27*B38*L35)/(J35*10^6)</f>
+        <f ca="1">(B27*B37*L34)/(J34*10^6)</f>
         <v>3.9551317414400003E-2</v>
       </c>
       <c r="C40" s="1">
@@ -2125,7 +2175,29 @@
         <v>39.551317414400003</v>
       </c>
       <c r="D40" s="1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A41" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="B41" s="1">
+        <f>(B38*B21)/(0.4*3.14*B19*100)</f>
+        <v>17.235723462999918</v>
+      </c>
+      <c r="C41" s="1"/>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A42" s="4" t="s">
         <v>148</v>
+      </c>
+      <c r="B42" s="1">
+        <f>B19*B41/B21</f>
+        <v>0.77229299363057324</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>138</v>
       </c>
     </row>
   </sheetData>
@@ -2147,7 +2219,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B96DE545-7F3F-4161-810A-0A86D0D5D381}">
   <dimension ref="A1:J39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A17" workbookViewId="0">
       <selection activeCell="O38" sqref="O38"/>
     </sheetView>
   </sheetViews>
@@ -2159,53 +2231,53 @@
   <sheetData>
     <row r="1" spans="1:10" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A1" s="30" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D1" s="30" t="s">
+        <v>50</v>
+      </c>
+      <c r="E1" s="30" t="s">
+        <v>51</v>
+      </c>
+      <c r="F1" s="30" t="s">
         <v>52</v>
       </c>
-      <c r="E1" s="30" t="s">
+      <c r="G1" s="30" t="s">
         <v>53</v>
       </c>
-      <c r="F1" s="30" t="s">
+      <c r="H1" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="G1" s="30" t="s">
-        <v>55</v>
-      </c>
-      <c r="H1" s="11" t="s">
+      <c r="I1" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="J1" s="30" t="s">
         <v>58</v>
-      </c>
-      <c r="J1" s="30" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="35.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="31"/>
       <c r="B2" s="12" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D2" s="31"/>
       <c r="E2" s="31"/>
       <c r="F2" s="31"/>
       <c r="G2" s="31"/>
       <c r="H2" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="I2" s="12" t="s">
         <v>57</v>
-      </c>
-      <c r="I2" s="12" t="s">
-        <v>59</v>
       </c>
       <c r="J2" s="31"/>
     </row>
@@ -2235,10 +2307,10 @@
         <v>302</v>
       </c>
       <c r="I3" s="13" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="J3" s="13" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
@@ -2267,10 +2339,10 @@
         <v>239</v>
       </c>
       <c r="I4" s="13" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="J4" s="13" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
@@ -2299,10 +2371,10 @@
         <v>190</v>
       </c>
       <c r="I5" s="13" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="J5" s="13" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
@@ -2331,10 +2403,10 @@
         <v>150</v>
       </c>
       <c r="I6" s="13" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="J6" s="13" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
@@ -2363,10 +2435,10 @@
         <v>119</v>
       </c>
       <c r="I7" s="13" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="J7" s="13" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
@@ -2395,10 +2467,10 @@
         <v>94</v>
       </c>
       <c r="I8" s="13" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="J8" s="13" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
@@ -2427,10 +2499,10 @@
         <v>75</v>
       </c>
       <c r="I9" s="13" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="J9" s="13" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
@@ -2459,10 +2531,10 @@
         <v>60</v>
       </c>
       <c r="I10" s="13" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="J10" s="13" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
@@ -2491,10 +2563,10 @@
         <v>47</v>
       </c>
       <c r="I11" s="13" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="J11" s="13" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
@@ -2523,10 +2595,10 @@
         <v>37</v>
       </c>
       <c r="I12" s="13" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="J12" s="13" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
@@ -2555,10 +2627,10 @@
         <v>30</v>
       </c>
       <c r="I13" s="13" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="J13" s="13" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
@@ -2587,10 +2659,10 @@
         <v>24</v>
       </c>
       <c r="I14" s="13" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="J14" s="13" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
@@ -2619,10 +2691,10 @@
         <v>19</v>
       </c>
       <c r="I15" s="13" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="J15" s="13" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
@@ -2651,10 +2723,10 @@
         <v>15</v>
       </c>
       <c r="I16" s="13" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="J16" s="13" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
@@ -2683,10 +2755,10 @@
         <v>12</v>
       </c>
       <c r="I17" s="13" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="J17" s="13" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
@@ -2715,10 +2787,10 @@
         <v>9.3000000000000007</v>
       </c>
       <c r="I18" s="13" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="J18" s="13" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
@@ -2747,10 +2819,10 @@
         <v>7.4</v>
       </c>
       <c r="I19" s="13" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="J19" s="13" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
@@ -2779,10 +2851,10 @@
         <v>5.9</v>
       </c>
       <c r="I20" s="13" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="J20" s="13" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.3">
@@ -2811,10 +2883,10 @@
         <v>4.7</v>
       </c>
       <c r="I21" s="13" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="J21" s="13" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
@@ -2843,10 +2915,10 @@
         <v>3.7</v>
       </c>
       <c r="I22" s="13" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="J22" s="13" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.3">
@@ -2875,10 +2947,10 @@
         <v>2.9</v>
       </c>
       <c r="I23" s="13" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="J23" s="13" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.3">
@@ -2907,10 +2979,10 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="I24" s="13" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="J24" s="13" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.3">
@@ -2939,10 +3011,10 @@
         <v>1.8</v>
       </c>
       <c r="I25" s="13" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="J25" s="13" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.3">
@@ -2971,10 +3043,10 @@
         <v>1.5</v>
       </c>
       <c r="I26" s="13" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="J26" s="13" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.3">
@@ -3003,10 +3075,10 @@
         <v>1.2</v>
       </c>
       <c r="I27" s="13" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="J27" s="13" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.3">
@@ -3035,10 +3107,10 @@
         <v>0.92</v>
       </c>
       <c r="I28" s="13" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="J28" s="13" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.3">
@@ -3067,10 +3139,10 @@
         <v>0.72899999999999998</v>
       </c>
       <c r="I29" s="13" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="J29" s="13" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.3">
@@ -3099,10 +3171,10 @@
         <v>0.57699999999999996</v>
       </c>
       <c r="I30" s="13" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="J30" s="13" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.3">
@@ -3131,10 +3203,10 @@
         <v>0.45700000000000002</v>
       </c>
       <c r="I31" s="13" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="J31" s="13" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.3">
@@ -3163,10 +3235,10 @@
         <v>0.36099999999999999</v>
       </c>
       <c r="I32" s="13" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="J32" s="13" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.3">
@@ -3195,10 +3267,10 @@
         <v>0.28799999999999998</v>
       </c>
       <c r="I33" s="13" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="J33" s="13" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.3">
@@ -3227,10 +3299,10 @@
         <v>0.22600000000000001</v>
       </c>
       <c r="I34" s="13" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="J34" s="13" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.3">
@@ -3259,10 +3331,10 @@
         <v>0.182</v>
       </c>
       <c r="I35" s="13" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="J35" s="13" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.3">
@@ -3291,10 +3363,10 @@
         <v>0.14199999999999999</v>
       </c>
       <c r="I36" s="13" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="J36" s="13" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.3">
@@ -3323,10 +3395,10 @@
         <v>0.113</v>
       </c>
       <c r="I37" s="13" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="J37" s="13" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.3">
@@ -3355,15 +3427,15 @@
         <v>9.0999999999999998E-2</v>
       </c>
       <c r="I38" s="13" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="J38" s="13" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="39" spans="1:10" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A39" s="16" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B39" s="13">
         <v>7.8700000000000003E-3</v>
@@ -3387,7 +3459,7 @@
         <v>8.7999999999999995E-2</v>
       </c>
       <c r="I39" s="13" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="J39" s="13"/>
     </row>
@@ -3425,7 +3497,7 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{27D7E5FF-15EE-4F2A-872A-6A49A9D7F096}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6E4D60C8-CCBE-474A-BD21-0A17B03580D5}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
     <ds:schemaRef ds:uri="http://www.boldonjames.com/2008/01/sie/internal/label"/>

</xml_diff>

<commit_message>
Magnetic Design Report Update
</commit_message>
<xml_diff>
--- a/Magnetic Design/Transformer_Design_Excel.xlsx
+++ b/Magnetic Design/Transformer_Design_Excel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahmetcan.akuz\Documents\GitHub\Optimus-Primary-Winding\Magnetic Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4064970-67D8-43DD-841F-F16BE05031D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEF35984-C583-43FE-AA95-6E40E5EEB0C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="13776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-90" yWindow="0" windowWidth="19380" windowHeight="20970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Transformer_Design" sheetId="1" r:id="rId1"/>
@@ -1615,8 +1615,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M39" sqref="M39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3497,7 +3497,7 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6E4D60C8-CCBE-474A-BD21-0A17B03580D5}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F5CA2540-F051-414D-B880-229370438C30}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
     <ds:schemaRef ds:uri="http://www.boldonjames.com/2008/01/sie/internal/label"/>

</xml_diff>

<commit_message>
Magnetic Design Report Updated
</commit_message>
<xml_diff>
--- a/Magnetic Design/Transformer_Design_Excel.xlsx
+++ b/Magnetic Design/Transformer_Design_Excel.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahmetcan.akuz\Documents\GitHub\Optimus-Primary-Winding\Magnetic Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEF35984-C583-43FE-AA95-6E40E5EEB0C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8380CFD7-E8C1-4B3F-9BCE-B52F27785A55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="0" windowWidth="19380" windowHeight="20970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Transformer_Design" sheetId="1" r:id="rId1"/>
     <sheet name="AWG" sheetId="3" r:id="rId2"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -60,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="157">
   <si>
     <t>Voltage Pri Min</t>
   </si>
@@ -522,6 +523,27 @@
   </si>
   <si>
     <t>Permiability, u (ungapped)</t>
+  </si>
+  <si>
+    <t>Steinmetz Coeff</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>Volume</t>
+  </si>
+  <si>
+    <t>Core loss</t>
+  </si>
+  <si>
+    <t>Copper Loss</t>
   </si>
 </sst>
 </file>
@@ -602,7 +624,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="18">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -813,12 +835,25 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -893,6 +928,7 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Check Cell" xfId="1" builtinId="23"/>
@@ -922,7 +958,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>174179</xdr:colOff>
+      <xdr:colOff>177989</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>35340</xdr:rowOff>
     </xdr:to>
@@ -971,7 +1007,7 @@
       <xdr:col>12</xdr:col>
       <xdr:colOff>225620</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>168671</xdr:rowOff>
+      <xdr:rowOff>172481</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1013,9 +1049,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>212263</xdr:colOff>
+      <xdr:colOff>216073</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>98067</xdr:rowOff>
+      <xdr:rowOff>101877</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1057,9 +1093,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>545631</xdr:colOff>
+      <xdr:colOff>553251</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>92237</xdr:rowOff>
+      <xdr:rowOff>96047</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1103,7 +1139,7 @@
       <xdr:col>17</xdr:col>
       <xdr:colOff>225523</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>128291</xdr:rowOff>
+      <xdr:rowOff>137181</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1147,7 +1183,7 @@
       <xdr:col>8</xdr:col>
       <xdr:colOff>378538</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>65442</xdr:rowOff>
+      <xdr:rowOff>62902</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1189,9 +1225,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>121919</xdr:colOff>
+      <xdr:colOff>135889</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>68580</xdr:rowOff>
+      <xdr:rowOff>62230</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1226,16 +1262,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>7620</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>160020</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>518160</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>175260</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>533565</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>30548</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>434505</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>39438</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1258,8 +1294,52 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4290060" y="6979920"/>
-          <a:ext cx="1905165" cy="784928"/>
+          <a:off x="5669280" y="6812280"/>
+          <a:ext cx="1905165" cy="778578"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>586740</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>31750</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>581419</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>20381</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{702207CF-3ED4-9D93-8D23-D5524BC9B15D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5737860" y="7948930"/>
+          <a:ext cx="1983499" cy="537271"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1613,10 +1693,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P42"/>
+  <dimension ref="A1:P46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M39" sqref="M39"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="M41" sqref="M41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1624,7 +1704,7 @@
     <col min="1" max="1" width="23.77734375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.44140625" customWidth="1"/>
-    <col min="4" max="4" width="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.77734375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.109375" customWidth="1"/>
     <col min="7" max="7" width="11.21875" customWidth="1"/>
     <col min="14" max="14" width="12" bestFit="1" customWidth="1"/>
@@ -1824,7 +1904,7 @@
         <v>20</v>
       </c>
       <c r="B18" s="1">
-        <v>0.3</v>
+        <v>0.27</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>22</v>
@@ -1906,7 +1986,7 @@
       </c>
       <c r="B23" s="1">
         <f>(B22*B13*10^6)/(B18*B19)</f>
-        <v>3.5765379113018603</v>
+        <v>3.9739310125576219</v>
       </c>
       <c r="C23" s="1"/>
     </row>
@@ -2189,15 +2269,73 @@
       <c r="C41" s="1"/>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A42" s="4" t="s">
+      <c r="A42" s="6" t="s">
         <v>148</v>
       </c>
-      <c r="B42" s="1">
+      <c r="B42" s="7">
         <f>B19*B41/B21</f>
         <v>0.77229299363057324</v>
       </c>
-      <c r="C42" s="1" t="s">
+      <c r="C42" s="7" t="s">
         <v>138</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A43" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A44" s="1"/>
+      <c r="B44" s="1">
+        <v>3.5301024810000001</v>
+      </c>
+      <c r="C44" s="1">
+        <v>1.4199999679999999</v>
+      </c>
+      <c r="D44" s="1">
+        <v>2.8849999359999998</v>
+      </c>
+      <c r="E44" s="1">
+        <v>5.1289999999999996</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A45" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="B45" s="1">
+        <f>((B44*((B6)^C44)*((B18)^D44))*E44)/10^6</f>
+        <v>2.5251031932306423</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D45" s="32"/>
+      <c r="E45" s="1"/>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A46" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="B46" s="1">
+        <f ca="1">B39*(B15^2)+B40*(B29^2)</f>
+        <v>0.29195897514666669</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -2219,8 +2357,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B96DE545-7F3F-4161-810A-0A86D0D5D381}">
   <dimension ref="A1:J39"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="O38" sqref="O38"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21:J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3492,12 +3630,471 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{848C375A-A1B7-4EB1-A0F7-C2B99C9A8D8E}">
+  <dimension ref="F10:O23"/>
+  <sheetViews>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10:O23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="10" spans="6:15" ht="30.6" x14ac:dyDescent="0.3">
+      <c r="F10" s="30" t="s">
+        <v>46</v>
+      </c>
+      <c r="G10" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="H10" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="I10" s="30" t="s">
+        <v>50</v>
+      </c>
+      <c r="J10" s="30" t="s">
+        <v>51</v>
+      </c>
+      <c r="K10" s="30" t="s">
+        <v>52</v>
+      </c>
+      <c r="L10" s="30" t="s">
+        <v>53</v>
+      </c>
+      <c r="M10" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="N10" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="O10" s="30" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="11" spans="6:15" ht="51" x14ac:dyDescent="0.3">
+      <c r="F11" s="31"/>
+      <c r="G11" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="H11" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="I11" s="31"/>
+      <c r="J11" s="31"/>
+      <c r="K11" s="31"/>
+      <c r="L11" s="31"/>
+      <c r="M11" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="N11" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="O11" s="31"/>
+    </row>
+    <row r="12" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="F12" s="16">
+        <v>15</v>
+      </c>
+      <c r="G12" s="13">
+        <v>5.7099999999999998E-2</v>
+      </c>
+      <c r="H12" s="15">
+        <v>1.45034</v>
+      </c>
+      <c r="I12" s="15">
+        <v>1.65</v>
+      </c>
+      <c r="J12" s="13">
+        <v>3.1840000000000002</v>
+      </c>
+      <c r="K12" s="13">
+        <v>10.443519999999999</v>
+      </c>
+      <c r="L12" s="13">
+        <v>28</v>
+      </c>
+      <c r="M12" s="13">
+        <v>4.7</v>
+      </c>
+      <c r="N12" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="O12" s="13" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="13" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="F13" s="16">
+        <v>16</v>
+      </c>
+      <c r="G13" s="13">
+        <v>5.0799999999999998E-2</v>
+      </c>
+      <c r="H13" s="15">
+        <v>1.2903199999999999</v>
+      </c>
+      <c r="I13" s="15">
+        <v>1.31</v>
+      </c>
+      <c r="J13" s="13">
+        <v>4.016</v>
+      </c>
+      <c r="K13" s="13">
+        <v>13.17248</v>
+      </c>
+      <c r="L13" s="13">
+        <v>22</v>
+      </c>
+      <c r="M13" s="13">
+        <v>3.7</v>
+      </c>
+      <c r="N13" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="O13" s="13" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="14" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="F14" s="16">
+        <v>17</v>
+      </c>
+      <c r="G14" s="13">
+        <v>4.53E-2</v>
+      </c>
+      <c r="H14" s="15">
+        <v>1.15062</v>
+      </c>
+      <c r="I14" s="15">
+        <v>1.04</v>
+      </c>
+      <c r="J14" s="13">
+        <v>5.0640000000000001</v>
+      </c>
+      <c r="K14" s="13">
+        <v>16.609919999999999</v>
+      </c>
+      <c r="L14" s="13">
+        <v>19</v>
+      </c>
+      <c r="M14" s="13">
+        <v>2.9</v>
+      </c>
+      <c r="N14" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="O14" s="13" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="F15" s="16">
+        <v>18</v>
+      </c>
+      <c r="G15" s="13">
+        <v>4.0300000000000002E-2</v>
+      </c>
+      <c r="H15" s="15">
+        <v>1.02362</v>
+      </c>
+      <c r="I15" s="15">
+        <v>0.82299999999999995</v>
+      </c>
+      <c r="J15" s="13">
+        <v>6.3849999999999998</v>
+      </c>
+      <c r="K15" s="13">
+        <v>20.942799999999998</v>
+      </c>
+      <c r="L15" s="13">
+        <v>16</v>
+      </c>
+      <c r="M15" s="13">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="N15" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="O15" s="13" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="16" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="F16" s="16">
+        <v>19</v>
+      </c>
+      <c r="G16" s="13">
+        <v>3.5900000000000001E-2</v>
+      </c>
+      <c r="H16" s="15">
+        <v>0.91186</v>
+      </c>
+      <c r="I16" s="15">
+        <v>0.65300000000000002</v>
+      </c>
+      <c r="J16" s="13">
+        <v>8.0510000000000002</v>
+      </c>
+      <c r="K16" s="13">
+        <v>26.40728</v>
+      </c>
+      <c r="L16" s="13">
+        <v>14</v>
+      </c>
+      <c r="M16" s="13">
+        <v>1.8</v>
+      </c>
+      <c r="N16" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="O16" s="13" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="17" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="F17" s="16">
+        <v>20</v>
+      </c>
+      <c r="G17" s="13">
+        <v>3.2000000000000001E-2</v>
+      </c>
+      <c r="H17" s="15">
+        <v>0.81279999999999997</v>
+      </c>
+      <c r="I17" s="15">
+        <v>0.51900000000000002</v>
+      </c>
+      <c r="J17" s="13">
+        <v>10.15</v>
+      </c>
+      <c r="K17" s="13">
+        <v>33.292000000000002</v>
+      </c>
+      <c r="L17" s="13">
+        <v>11</v>
+      </c>
+      <c r="M17" s="13">
+        <v>1.5</v>
+      </c>
+      <c r="N17" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="O17" s="13" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="18" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="F18" s="16">
+        <v>21</v>
+      </c>
+      <c r="G18" s="13">
+        <v>2.8500000000000001E-2</v>
+      </c>
+      <c r="H18" s="15">
+        <v>0.72389999999999999</v>
+      </c>
+      <c r="I18" s="15">
+        <v>0.41199999999999998</v>
+      </c>
+      <c r="J18" s="13">
+        <v>12.8</v>
+      </c>
+      <c r="K18" s="13">
+        <v>41.984000000000002</v>
+      </c>
+      <c r="L18" s="13">
+        <v>9</v>
+      </c>
+      <c r="M18" s="13">
+        <v>1.2</v>
+      </c>
+      <c r="N18" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="O18" s="13" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="19" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="F19" s="16">
+        <v>22</v>
+      </c>
+      <c r="G19" s="13">
+        <v>2.53E-2</v>
+      </c>
+      <c r="H19" s="15">
+        <v>0.64515999999999996</v>
+      </c>
+      <c r="I19" s="15">
+        <v>0.32700000000000001</v>
+      </c>
+      <c r="J19" s="13">
+        <v>16.14</v>
+      </c>
+      <c r="K19" s="13">
+        <v>52.9392</v>
+      </c>
+      <c r="L19" s="13">
+        <v>7</v>
+      </c>
+      <c r="M19" s="13">
+        <v>0.92</v>
+      </c>
+      <c r="N19" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="O19" s="13" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="20" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="F20" s="16">
+        <v>23</v>
+      </c>
+      <c r="G20" s="13">
+        <v>2.2599999999999999E-2</v>
+      </c>
+      <c r="H20" s="15">
+        <v>0.57403999999999999</v>
+      </c>
+      <c r="I20" s="15">
+        <v>0.25900000000000001</v>
+      </c>
+      <c r="J20" s="13">
+        <v>20.36</v>
+      </c>
+      <c r="K20" s="13">
+        <v>66.780799999999999</v>
+      </c>
+      <c r="L20" s="13">
+        <v>4.7</v>
+      </c>
+      <c r="M20" s="13">
+        <v>0.72899999999999998</v>
+      </c>
+      <c r="N20" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="O20" s="13" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="21" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="F21" s="16">
+        <v>24</v>
+      </c>
+      <c r="G21" s="13">
+        <v>2.01E-2</v>
+      </c>
+      <c r="H21" s="15">
+        <v>0.51053999999999999</v>
+      </c>
+      <c r="I21" s="15">
+        <v>0.20499999999999999</v>
+      </c>
+      <c r="J21" s="13">
+        <v>25.67</v>
+      </c>
+      <c r="K21" s="13">
+        <v>84.197599999999994</v>
+      </c>
+      <c r="L21" s="13">
+        <v>3.5</v>
+      </c>
+      <c r="M21" s="13">
+        <v>0.57699999999999996</v>
+      </c>
+      <c r="N21" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="O21" s="13" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="22" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="F22" s="16">
+        <v>25</v>
+      </c>
+      <c r="G22" s="13">
+        <v>1.7899999999999999E-2</v>
+      </c>
+      <c r="H22" s="15">
+        <v>0.45466000000000001</v>
+      </c>
+      <c r="I22" s="15">
+        <v>0.16200000000000001</v>
+      </c>
+      <c r="J22" s="13">
+        <v>32.369999999999997</v>
+      </c>
+      <c r="K22" s="13">
+        <v>106.17359999999999</v>
+      </c>
+      <c r="L22" s="13">
+        <v>2.7</v>
+      </c>
+      <c r="M22" s="13">
+        <v>0.45700000000000002</v>
+      </c>
+      <c r="N22" s="13" t="s">
+        <v>115</v>
+      </c>
+      <c r="O22" s="13" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="23" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="F23" s="16">
+        <v>26</v>
+      </c>
+      <c r="G23" s="13">
+        <v>1.5900000000000001E-2</v>
+      </c>
+      <c r="H23" s="15">
+        <v>0.40386</v>
+      </c>
+      <c r="I23" s="15">
+        <v>0.128</v>
+      </c>
+      <c r="J23" s="13">
+        <v>40.81</v>
+      </c>
+      <c r="K23" s="13">
+        <v>133.85679999999999</v>
+      </c>
+      <c r="L23" s="13">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="M23" s="13">
+        <v>0.36099999999999999</v>
+      </c>
+      <c r="N23" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="O23" s="13" t="s">
+        <v>118</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="O10:O11"/>
+    <mergeCell ref="F10:F11"/>
+    <mergeCell ref="I10:I11"/>
+    <mergeCell ref="J10:J11"/>
+    <mergeCell ref="K10:K11"/>
+    <mergeCell ref="L10:L11"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
 <sisl xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns="http://www.boldonjames.com/2008/01/sie/internal/label" sislVersion="0" policy="0399a3f6-84a2-44f7-8781-b1ee60ec893b" origin="userSelected"/>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F5CA2540-F051-414D-B880-229370438C30}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DAAB3985-EB40-4E8E-BD2F-37518C31538B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
     <ds:schemaRef ds:uri="http://www.boldonjames.com/2008/01/sie/internal/label"/>

</xml_diff>

<commit_message>
Presentation added, Excel Updated
</commit_message>
<xml_diff>
--- a/Magnetic Design/Transformer_Design_Excel.xlsx
+++ b/Magnetic Design/Transformer_Design_Excel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahmetcan.akuz\Documents\GitHub\Optimus-Primary-Winding\Magnetic Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8380CFD7-E8C1-4B3F-9BCE-B52F27785A55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3843B4D1-67EF-4984-9018-A3CB37E80367}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23148" yWindow="11364" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Transformer_Design" sheetId="1" r:id="rId1"/>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="156">
   <si>
     <t>Voltage Pri Min</t>
   </si>
@@ -507,12 +507,6 @@
     <t>R_sec</t>
   </si>
   <si>
-    <t>resis_pri</t>
-  </si>
-  <si>
-    <t>resis_sec</t>
-  </si>
-  <si>
     <t>mOhm</t>
   </si>
   <si>
@@ -544,6 +538,9 @@
   </si>
   <si>
     <t>Copper Loss</t>
+  </si>
+  <si>
+    <t>Ohm/m</t>
   </si>
 </sst>
 </file>
@@ -853,7 +850,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -883,6 +880,7 @@
     <xf numFmtId="0" fontId="4" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -928,7 +926,8 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Check Cell" xfId="1" builtinId="23"/>
@@ -958,7 +957,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>177989</xdr:colOff>
+      <xdr:colOff>174179</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>35340</xdr:rowOff>
     </xdr:to>
@@ -1007,7 +1006,7 @@
       <xdr:col>12</xdr:col>
       <xdr:colOff>225620</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>172481</xdr:rowOff>
+      <xdr:rowOff>175021</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1049,9 +1048,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>216073</xdr:colOff>
+      <xdr:colOff>212263</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>101877</xdr:rowOff>
+      <xdr:rowOff>98067</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1093,9 +1092,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>553251</xdr:colOff>
+      <xdr:colOff>555791</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>96047</xdr:rowOff>
+      <xdr:rowOff>98587</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1139,7 +1138,7 @@
       <xdr:col>17</xdr:col>
       <xdr:colOff>225523</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>137181</xdr:rowOff>
+      <xdr:rowOff>139721</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1183,7 +1182,7 @@
       <xdr:col>8</xdr:col>
       <xdr:colOff>378538</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>62902</xdr:rowOff>
+      <xdr:rowOff>59092</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1225,9 +1224,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>135889</xdr:colOff>
+      <xdr:colOff>138429</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>62230</xdr:rowOff>
+      <xdr:rowOff>58420</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1269,7 +1268,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>434505</xdr:colOff>
+      <xdr:colOff>442125</xdr:colOff>
       <xdr:row>40</xdr:row>
       <xdr:rowOff>39438</xdr:rowOff>
     </xdr:to>
@@ -1313,9 +1312,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>581419</xdr:colOff>
+      <xdr:colOff>592849</xdr:colOff>
       <xdr:row>45</xdr:row>
-      <xdr:rowOff>20381</xdr:rowOff>
+      <xdr:rowOff>22921</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1695,29 +1694,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="M41" sqref="M41"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="23.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.44140625" customWidth="1"/>
-    <col min="4" max="4" width="11.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.109375" customWidth="1"/>
-    <col min="7" max="7" width="11.21875" customWidth="1"/>
+    <col min="1" max="1" width="23.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.453125" customWidth="1"/>
+    <col min="4" max="4" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.08984375" customWidth="1"/>
+    <col min="7" max="7" width="11.1796875" customWidth="1"/>
     <col min="14" max="14" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="18" t="s">
+    <row r="1" spans="1:16" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="20"/>
-    </row>
-    <row r="2" spans="1:16" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="20"/>
+      <c r="C1" s="21"/>
+    </row>
+    <row r="2" spans="1:16" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1728,7 +1727,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -1739,7 +1738,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -1750,7 +1749,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
@@ -1759,7 +1758,7 @@
       </c>
       <c r="C5" s="1"/>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
@@ -1770,7 +1769,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
@@ -1782,7 +1781,7 @@
       </c>
       <c r="K7" s="3"/>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>16</v>
       </c>
@@ -1793,7 +1792,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>15</v>
       </c>
@@ -1806,14 +1805,14 @@
       <c r="F9" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="G9" s="27" t="s">
+      <c r="G9" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="H9" s="27"/>
-      <c r="I9" s="27"/>
-      <c r="J9" s="27"/>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="H9" s="28"/>
+      <c r="I9" s="28"/>
+      <c r="J9" s="28"/>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A10" s="10" t="s">
         <v>40</v>
       </c>
@@ -1822,14 +1821,14 @@
       </c>
       <c r="C10" s="1"/>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A11" s="21" t="s">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A11" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="22"/>
-      <c r="C11" s="23"/>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="B11" s="23"/>
+      <c r="C11" s="24"/>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
         <v>12</v>
       </c>
@@ -1841,7 +1840,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
         <v>14</v>
       </c>
@@ -1853,7 +1852,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="s">
         <v>11</v>
       </c>
@@ -1875,7 +1874,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A15" s="4" t="s">
         <v>24</v>
       </c>
@@ -1887,19 +1886,19 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A16" s="4"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A17" s="24" t="s">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A17" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="25"/>
-      <c r="C17" s="26"/>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B17" s="26"/>
+      <c r="C17" s="27"/>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
         <v>20</v>
       </c>
@@ -1919,7 +1918,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
         <v>21</v>
       </c>
@@ -1930,18 +1929,18 @@
         <v>23</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
         <v>41</v>
       </c>
       <c r="B20" s="5">
-        <v>374</v>
+        <v>341</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="21" spans="1:14" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:14" ht="31.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
         <v>36</v>
       </c>
@@ -1951,16 +1950,16 @@
       <c r="C21" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D21" s="28" t="s">
+      <c r="D21" s="29" t="s">
         <v>140</v>
       </c>
-      <c r="E21" s="28"/>
-      <c r="F21" s="29" t="s">
+      <c r="E21" s="29"/>
+      <c r="F21" s="30" t="s">
         <v>139</v>
       </c>
-      <c r="G21" s="29"/>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="G21" s="30"/>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A22" s="4" t="s">
         <v>26</v>
       </c>
@@ -1980,7 +1979,7 @@
       </c>
       <c r="F22" s="9"/>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A23" s="4" t="s">
         <v>28</v>
       </c>
@@ -1990,7 +1989,7 @@
       </c>
       <c r="C23" s="1"/>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A24" s="4" t="s">
         <v>27</v>
       </c>
@@ -2000,7 +1999,7 @@
       </c>
       <c r="C24" s="1"/>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A25" s="4" t="s">
         <v>31</v>
       </c>
@@ -2009,8 +2008,12 @@
         <v>4</v>
       </c>
       <c r="C25" s="1"/>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="L25">
+        <f>64*0.2</f>
+        <v>12.8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A26" s="4" t="s">
         <v>32</v>
       </c>
@@ -2020,7 +2023,7 @@
       </c>
       <c r="C26" s="1"/>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A27" s="6" t="s">
         <v>33</v>
       </c>
@@ -2029,10 +2032,10 @@
         <v>16</v>
       </c>
       <c r="C27" s="7"/>
-      <c r="F27" s="17"/>
-      <c r="G27" s="17"/>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A28" s="4" t="s">
         <v>34</v>
       </c>
@@ -2048,7 +2051,7 @@
         <v>830.07812500000011</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A29" s="4" t="s">
         <v>35</v>
       </c>
@@ -2060,7 +2063,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A30" s="2" t="s">
         <v>38</v>
       </c>
@@ -2071,7 +2074,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A31" s="4" t="s">
         <v>42</v>
       </c>
@@ -2085,8 +2088,8 @@
       <c r="D31" s="8"/>
       <c r="F31" s="8"/>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A32" s="4" t="s">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A32" s="6" t="s">
         <v>43</v>
       </c>
       <c r="B32" s="7">
@@ -2097,7 +2100,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A33" s="2" t="s">
         <v>133</v>
       </c>
@@ -2131,15 +2134,18 @@
         <f ca="1">ROUNDUP(B31/D33,0)</f>
         <v>8</v>
       </c>
-      <c r="K33" s="1" t="s">
-        <v>144</v>
+      <c r="K33" s="4" t="s">
+        <v>142</v>
       </c>
       <c r="L33" s="1" cm="1">
-        <f t="array" aca="1" ref="L33" ca="1">INDIRECT("AWG!F" &amp; B33+6)</f>
-        <v>84.197599999999994</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+        <f t="array" aca="1" ref="L33" ca="1">INDIRECT("AWG!F" &amp; B33+6)/1000</f>
+        <v>8.4197599999999997E-2</v>
+      </c>
+      <c r="M33" s="34" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A34" s="2" t="s">
         <v>135</v>
       </c>
@@ -2173,16 +2179,19 @@
         <f ca="1">ROUNDUP(B32/D34,0)</f>
         <v>2</v>
       </c>
-      <c r="K34" s="1" t="s">
-        <v>145</v>
+      <c r="K34" s="4" t="s">
+        <v>143</v>
       </c>
       <c r="L34" s="1" cm="1">
-        <f t="array" aca="1" ref="L34" ca="1">INDIRECT("AWG!F" &amp; B34+6)</f>
-        <v>84.197599999999994</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A35" s="4" t="s">
+        <f t="array" aca="1" ref="L34" ca="1">INDIRECT("AWG!F" &amp; B34+6)/1000</f>
+        <v>8.4197599999999997E-2</v>
+      </c>
+      <c r="M34" s="34" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A35" s="33" t="s">
         <v>44</v>
       </c>
       <c r="B35" s="14">
@@ -2193,17 +2202,17 @@
         <v>23</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A36" s="6" t="s">
         <v>45</v>
       </c>
       <c r="B36" s="7">
         <f ca="1">B35/B20</f>
-        <v>3.5080213903743315E-2</v>
+        <v>3.8475073313782991E-2</v>
       </c>
       <c r="C36" s="7"/>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A37" s="2" t="s">
         <v>141</v>
       </c>
@@ -2211,12 +2220,14 @@
         <f>2*3.14*(30.9-12.2)/2</f>
         <v>58.718000000000004</v>
       </c>
-      <c r="C37" s="1"/>
+      <c r="C37" s="1" t="s">
+        <v>138</v>
+      </c>
       <c r="D37" s="1"/>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A38" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B38" s="1">
         <v>97</v>
@@ -2226,12 +2237,12 @@
       </c>
       <c r="D38" s="1"/>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A39" s="4" t="s">
         <v>142</v>
       </c>
       <c r="B39" s="1">
-        <f ca="1">(B25*B37*L33)/(J33*10^6)</f>
+        <f ca="1">(B25*B37*L33)/(J33*10^3)</f>
         <v>2.4719573384000002E-3</v>
       </c>
       <c r="C39" s="1">
@@ -2239,15 +2250,15 @@
         <v>2.4719573384000002</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A40" s="4" t="s">
         <v>143</v>
       </c>
       <c r="B40" s="1">
-        <f ca="1">(B27*B37*L34)/(J34*10^6)</f>
+        <f ca="1">(B27*B37*L34)/(J34*10^3)</f>
         <v>3.9551317414400003E-2</v>
       </c>
       <c r="C40" s="1">
@@ -2255,49 +2266,49 @@
         <v>39.551317414400003</v>
       </c>
       <c r="D40" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A41" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="B41" s="1">
+        <f>(B38*B21)/(0.4*3.14*B19*10)</f>
+        <v>172.35723462999914</v>
+      </c>
+      <c r="C41" s="1"/>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A42" s="6" t="s">
         <v>146</v>
-      </c>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A41" s="4" t="s">
-        <v>149</v>
-      </c>
-      <c r="B41" s="1">
-        <f>(B38*B21)/(0.4*3.14*B19*100)</f>
-        <v>17.235723462999918</v>
-      </c>
-      <c r="C41" s="1"/>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A42" s="6" t="s">
-        <v>148</v>
       </c>
       <c r="B42" s="7">
         <f>B19*B41/B21</f>
-        <v>0.77229299363057324</v>
+        <v>7.7229299363057304</v>
       </c>
       <c r="C42" s="7" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A43" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="C43" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="B43" s="2" t="s">
+      <c r="D43" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="C43" s="2" t="s">
+      <c r="E43" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="D43" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="E43" s="2" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A44" s="1"/>
       <c r="B44" s="1">
         <v>3.5301024810000001</v>
@@ -2312,9 +2323,9 @@
         <v>5.1289999999999996</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A45" s="4" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B45" s="1">
         <f>((B44*((B6)^C44)*((B18)^D44))*E44)/10^6</f>
@@ -2323,12 +2334,12 @@
       <c r="C45" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D45" s="32"/>
+      <c r="D45" s="17"/>
       <c r="E45" s="1"/>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A46" s="4" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B46" s="1">
         <f ca="1">B39*(B15^2)+B40*(B29^2)</f>
@@ -2358,17 +2369,17 @@
   <dimension ref="A1:J39"/>
   <sheetViews>
     <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21:J21"/>
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="7.21875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.1796875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A1" s="30" t="s">
+    <row r="1" spans="1:10" ht="20" x14ac:dyDescent="0.35">
+      <c r="A1" s="31" t="s">
         <v>46</v>
       </c>
       <c r="B1" s="11" t="s">
@@ -2377,16 +2388,16 @@
       <c r="C1" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="D1" s="30" t="s">
+      <c r="D1" s="31" t="s">
         <v>50</v>
       </c>
-      <c r="E1" s="30" t="s">
+      <c r="E1" s="31" t="s">
         <v>51</v>
       </c>
-      <c r="F1" s="30" t="s">
+      <c r="F1" s="31" t="s">
         <v>52</v>
       </c>
-      <c r="G1" s="30" t="s">
+      <c r="G1" s="31" t="s">
         <v>53</v>
       </c>
       <c r="H1" s="11" t="s">
@@ -2395,31 +2406,31 @@
       <c r="I1" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="J1" s="30" t="s">
+      <c r="J1" s="31" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="35.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="31"/>
+    <row r="2" spans="1:10" ht="35.4" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="32"/>
       <c r="B2" s="12" t="s">
         <v>48</v>
       </c>
       <c r="C2" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
-      <c r="G2" s="31"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
       <c r="H2" s="12" t="s">
         <v>55</v>
       </c>
       <c r="I2" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="J2" s="31"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J2" s="32"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="16">
         <v>0</v>
       </c>
@@ -2451,7 +2462,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" s="16">
         <v>0</v>
       </c>
@@ -2483,7 +2494,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" s="16">
         <v>0</v>
       </c>
@@ -2515,7 +2526,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" s="16">
         <v>0</v>
       </c>
@@ -2547,7 +2558,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" s="16">
         <v>1</v>
       </c>
@@ -2579,7 +2590,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" s="16">
         <v>2</v>
       </c>
@@ -2611,7 +2622,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" s="16">
         <v>3</v>
       </c>
@@ -2643,7 +2654,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" s="16">
         <v>4</v>
       </c>
@@ -2675,7 +2686,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" s="16">
         <v>5</v>
       </c>
@@ -2707,7 +2718,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12" s="16">
         <v>6</v>
       </c>
@@ -2739,7 +2750,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13" s="16">
         <v>7</v>
       </c>
@@ -2771,7 +2782,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14" s="16">
         <v>8</v>
       </c>
@@ -2803,7 +2814,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15" s="16">
         <v>9</v>
       </c>
@@ -2835,7 +2846,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A16" s="16">
         <v>10</v>
       </c>
@@ -2867,7 +2878,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A17" s="16">
         <v>11</v>
       </c>
@@ -2899,7 +2910,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A18" s="16">
         <v>12</v>
       </c>
@@ -2931,7 +2942,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A19" s="16">
         <v>13</v>
       </c>
@@ -2963,7 +2974,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A20" s="16">
         <v>14</v>
       </c>
@@ -2995,7 +3006,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A21" s="16">
         <v>15</v>
       </c>
@@ -3027,7 +3038,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A22" s="16">
         <v>16</v>
       </c>
@@ -3059,7 +3070,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A23" s="16">
         <v>17</v>
       </c>
@@ -3091,7 +3102,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A24" s="16">
         <v>18</v>
       </c>
@@ -3123,7 +3134,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A25" s="16">
         <v>19</v>
       </c>
@@ -3155,7 +3166,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A26" s="16">
         <v>20</v>
       </c>
@@ -3187,7 +3198,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A27" s="16">
         <v>21</v>
       </c>
@@ -3219,7 +3230,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A28" s="16">
         <v>22</v>
       </c>
@@ -3251,7 +3262,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A29" s="16">
         <v>23</v>
       </c>
@@ -3283,7 +3294,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A30" s="16">
         <v>24</v>
       </c>
@@ -3315,7 +3326,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A31" s="16">
         <v>25</v>
       </c>
@@ -3347,7 +3358,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A32" s="16">
         <v>26</v>
       </c>
@@ -3379,7 +3390,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A33" s="16">
         <v>27</v>
       </c>
@@ -3411,7 +3422,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A34" s="16">
         <v>28</v>
       </c>
@@ -3443,7 +3454,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A35" s="16">
         <v>29</v>
       </c>
@@ -3475,7 +3486,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A36" s="16">
         <v>30</v>
       </c>
@@ -3507,7 +3518,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A37" s="16">
         <v>31</v>
       </c>
@@ -3539,7 +3550,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A38" s="16">
         <v>32</v>
       </c>
@@ -3571,7 +3582,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="39" spans="1:10" ht="20.399999999999999" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:10" ht="21" x14ac:dyDescent="0.35">
       <c r="A39" s="16" t="s">
         <v>131</v>
       </c>
@@ -3623,7 +3634,7 @@
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -3638,10 +3649,10 @@
       <selection activeCell="F10" sqref="F10:O23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="10" spans="6:15" ht="30.6" x14ac:dyDescent="0.3">
-      <c r="F10" s="30" t="s">
+    <row r="10" spans="6:15" ht="30" x14ac:dyDescent="0.35">
+      <c r="F10" s="31" t="s">
         <v>46</v>
       </c>
       <c r="G10" s="11" t="s">
@@ -3650,16 +3661,16 @@
       <c r="H10" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="I10" s="30" t="s">
+      <c r="I10" s="31" t="s">
         <v>50</v>
       </c>
-      <c r="J10" s="30" t="s">
+      <c r="J10" s="31" t="s">
         <v>51</v>
       </c>
-      <c r="K10" s="30" t="s">
+      <c r="K10" s="31" t="s">
         <v>52</v>
       </c>
-      <c r="L10" s="30" t="s">
+      <c r="L10" s="31" t="s">
         <v>53</v>
       </c>
       <c r="M10" s="11" t="s">
@@ -3668,31 +3679,31 @@
       <c r="N10" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="O10" s="30" t="s">
+      <c r="O10" s="31" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="11" spans="6:15" ht="51" x14ac:dyDescent="0.3">
-      <c r="F11" s="31"/>
+    <row r="11" spans="6:15" ht="50" x14ac:dyDescent="0.35">
+      <c r="F11" s="32"/>
       <c r="G11" s="12" t="s">
         <v>48</v>
       </c>
       <c r="H11" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="I11" s="31"/>
-      <c r="J11" s="31"/>
-      <c r="K11" s="31"/>
-      <c r="L11" s="31"/>
+      <c r="I11" s="32"/>
+      <c r="J11" s="32"/>
+      <c r="K11" s="32"/>
+      <c r="L11" s="32"/>
       <c r="M11" s="12" t="s">
         <v>55</v>
       </c>
       <c r="N11" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="O11" s="31"/>
-    </row>
-    <row r="12" spans="6:15" x14ac:dyDescent="0.3">
+      <c r="O11" s="32"/>
+    </row>
+    <row r="12" spans="6:15" x14ac:dyDescent="0.35">
       <c r="F12" s="16">
         <v>15</v>
       </c>
@@ -3724,7 +3735,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="13" spans="6:15" x14ac:dyDescent="0.3">
+    <row r="13" spans="6:15" x14ac:dyDescent="0.35">
       <c r="F13" s="16">
         <v>16</v>
       </c>
@@ -3756,7 +3767,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="14" spans="6:15" x14ac:dyDescent="0.3">
+    <row r="14" spans="6:15" x14ac:dyDescent="0.35">
       <c r="F14" s="16">
         <v>17</v>
       </c>
@@ -3788,7 +3799,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="15" spans="6:15" x14ac:dyDescent="0.3">
+    <row r="15" spans="6:15" x14ac:dyDescent="0.35">
       <c r="F15" s="16">
         <v>18</v>
       </c>
@@ -3820,7 +3831,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="16" spans="6:15" x14ac:dyDescent="0.3">
+    <row r="16" spans="6:15" x14ac:dyDescent="0.35">
       <c r="F16" s="16">
         <v>19</v>
       </c>
@@ -3852,7 +3863,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="17" spans="6:15" x14ac:dyDescent="0.3">
+    <row r="17" spans="6:15" x14ac:dyDescent="0.35">
       <c r="F17" s="16">
         <v>20</v>
       </c>
@@ -3884,7 +3895,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="18" spans="6:15" x14ac:dyDescent="0.3">
+    <row r="18" spans="6:15" x14ac:dyDescent="0.35">
       <c r="F18" s="16">
         <v>21</v>
       </c>
@@ -3916,7 +3927,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="19" spans="6:15" x14ac:dyDescent="0.3">
+    <row r="19" spans="6:15" x14ac:dyDescent="0.35">
       <c r="F19" s="16">
         <v>22</v>
       </c>
@@ -3948,7 +3959,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="20" spans="6:15" x14ac:dyDescent="0.3">
+    <row r="20" spans="6:15" x14ac:dyDescent="0.35">
       <c r="F20" s="16">
         <v>23</v>
       </c>
@@ -3980,7 +3991,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="21" spans="6:15" x14ac:dyDescent="0.3">
+    <row r="21" spans="6:15" x14ac:dyDescent="0.35">
       <c r="F21" s="16">
         <v>24</v>
       </c>
@@ -4012,7 +4023,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="22" spans="6:15" x14ac:dyDescent="0.3">
+    <row r="22" spans="6:15" x14ac:dyDescent="0.35">
       <c r="F22" s="16">
         <v>25</v>
       </c>
@@ -4044,7 +4055,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="23" spans="6:15" x14ac:dyDescent="0.3">
+    <row r="23" spans="6:15" x14ac:dyDescent="0.35">
       <c r="F23" s="16">
         <v>26</v>
       </c>
@@ -4094,7 +4105,7 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DAAB3985-EB40-4E8E-BD2F-37518C31538B}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F014ECB5-640D-44E8-8278-F8A28E04C11C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
     <ds:schemaRef ds:uri="http://www.boldonjames.com/2008/01/sie/internal/label"/>

</xml_diff>

<commit_message>
Temp Rise Calculation Added
</commit_message>
<xml_diff>
--- a/Magnetic Design/Transformer_Design_Excel.xlsx
+++ b/Magnetic Design/Transformer_Design_Excel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahmetcan.akuz\Documents\GitHub\Optimus-Primary-Winding\Magnetic Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3843B4D1-67EF-4984-9018-A3CB37E80367}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D43EE4C-54A5-42D1-BA08-4E21A617F3E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="11364" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5260" yWindow="8140" windowWidth="24330" windowHeight="12210" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Transformer_Design" sheetId="1" r:id="rId1"/>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="164">
   <si>
     <t>Voltage Pri Min</t>
   </si>
@@ -542,12 +542,47 @@
   <si>
     <t>Ohm/m</t>
   </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>cm^2</t>
+  </si>
+  <si>
+    <t>Surface Area,At</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Temp Rise </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>∆T</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -581,6 +616,12 @@
       <sz val="8"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -850,7 +891,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -881,6 +922,7 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -926,8 +968,6 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Check Cell" xfId="1" builtinId="23"/>
@@ -957,7 +997,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>174179</xdr:colOff>
+      <xdr:colOff>172909</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>35340</xdr:rowOff>
     </xdr:to>
@@ -1006,7 +1046,7 @@
       <xdr:col>12</xdr:col>
       <xdr:colOff>225620</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>175021</xdr:rowOff>
+      <xdr:rowOff>173751</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1048,9 +1088,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>212263</xdr:colOff>
+      <xdr:colOff>210993</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>98067</xdr:rowOff>
+      <xdr:rowOff>96797</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1092,9 +1132,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>555791</xdr:colOff>
+      <xdr:colOff>554521</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>98587</xdr:rowOff>
+      <xdr:rowOff>97317</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1138,7 +1178,7 @@
       <xdr:col>17</xdr:col>
       <xdr:colOff>225523</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>139721</xdr:rowOff>
+      <xdr:rowOff>138451</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1182,7 +1222,7 @@
       <xdr:col>8</xdr:col>
       <xdr:colOff>378538</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>59092</xdr:rowOff>
+      <xdr:rowOff>57822</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1224,9 +1264,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>138429</xdr:colOff>
+      <xdr:colOff>137159</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>58420</xdr:rowOff>
+      <xdr:rowOff>63500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1268,7 +1308,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>442125</xdr:colOff>
+      <xdr:colOff>440855</xdr:colOff>
       <xdr:row>40</xdr:row>
       <xdr:rowOff>39438</xdr:rowOff>
     </xdr:to>
@@ -1312,9 +1352,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>592849</xdr:colOff>
+      <xdr:colOff>591579</xdr:colOff>
       <xdr:row>45</xdr:row>
-      <xdr:rowOff>22921</xdr:rowOff>
+      <xdr:rowOff>21651</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1692,10 +1732,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P46"/>
+  <dimension ref="A1:P54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="H57" sqref="H57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1710,11 +1750,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="21"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="22"/>
     </row>
     <row r="2" spans="1:16" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
@@ -1805,12 +1845,12 @@
       <c r="F9" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="G9" s="28" t="s">
+      <c r="G9" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="H9" s="28"/>
-      <c r="I9" s="28"/>
-      <c r="J9" s="28"/>
+      <c r="H9" s="29"/>
+      <c r="I9" s="29"/>
+      <c r="J9" s="29"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A10" s="10" t="s">
@@ -1822,11 +1862,11 @@
       <c r="C10" s="1"/>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A11" s="22" t="s">
+      <c r="A11" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="23"/>
-      <c r="C11" s="24"/>
+      <c r="B11" s="24"/>
+      <c r="C11" s="25"/>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
@@ -1892,11 +1932,11 @@
       <c r="C16" s="1"/>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A17" s="25" t="s">
+      <c r="A17" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="26"/>
-      <c r="C17" s="27"/>
+      <c r="B17" s="27"/>
+      <c r="C17" s="28"/>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
@@ -1950,14 +1990,14 @@
       <c r="C21" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D21" s="29" t="s">
+      <c r="D21" s="30" t="s">
         <v>140</v>
       </c>
-      <c r="E21" s="29"/>
-      <c r="F21" s="30" t="s">
+      <c r="E21" s="30"/>
+      <c r="F21" s="31" t="s">
         <v>139</v>
       </c>
-      <c r="G21" s="30"/>
+      <c r="G21" s="31"/>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A22" s="4" t="s">
@@ -2008,10 +2048,6 @@
         <v>4</v>
       </c>
       <c r="C25" s="1"/>
-      <c r="L25">
-        <f>64*0.2</f>
-        <v>12.8</v>
-      </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A26" s="4" t="s">
@@ -2032,8 +2068,8 @@
         <v>16</v>
       </c>
       <c r="C27" s="7"/>
-      <c r="F27" s="18"/>
-      <c r="G27" s="18"/>
+      <c r="F27" s="19"/>
+      <c r="G27" s="19"/>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A28" s="4" t="s">
@@ -2046,10 +2082,6 @@
       <c r="C28" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="I28">
-        <f>1000*D22/16</f>
-        <v>830.07812500000011</v>
-      </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A29" s="4" t="s">
@@ -2141,7 +2173,7 @@
         <f t="array" aca="1" ref="L33" ca="1">INDIRECT("AWG!F" &amp; B33+6)/1000</f>
         <v>8.4197599999999997E-2</v>
       </c>
-      <c r="M33" s="34" t="s">
+      <c r="M33" s="1" t="s">
         <v>155</v>
       </c>
     </row>
@@ -2186,12 +2218,12 @@
         <f t="array" aca="1" ref="L34" ca="1">INDIRECT("AWG!F" &amp; B34+6)/1000</f>
         <v>8.4197599999999997E-2</v>
       </c>
-      <c r="M34" s="34" t="s">
+      <c r="M34" s="1" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A35" s="33" t="s">
+      <c r="A35" s="18" t="s">
         <v>44</v>
       </c>
       <c r="B35" s="14">
@@ -2347,6 +2379,93 @@
       </c>
       <c r="C46" s="1" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A47" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B47" s="1">
+        <v>43</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A48" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="B48" s="1">
+        <v>30.9</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A49" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="B49" s="1">
+        <v>12.2</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A50" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="B50" s="1">
+        <v>21.2</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A51" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="B51" s="1">
+        <v>15.4</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A52" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="B52" s="1">
+        <v>20</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A53" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="B53" s="1">
+        <f>(2*B47*B52+(B51*B52*4)+2*B50*B52+2*(B47*B50-B51*(B48-B49)))/100</f>
+        <v>50.4724</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A54" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="B54" s="1">
+        <f ca="1">(((B45+B46)*1000/B53)^(0.833))</f>
+        <v>28.512577696779253</v>
       </c>
     </row>
   </sheetData>
@@ -2360,7 +2479,8 @@
     <mergeCell ref="F21:G21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -2379,7 +2499,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="20" x14ac:dyDescent="0.35">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="32" t="s">
         <v>46</v>
       </c>
       <c r="B1" s="11" t="s">
@@ -2388,16 +2508,16 @@
       <c r="C1" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="D1" s="31" t="s">
+      <c r="D1" s="32" t="s">
         <v>50</v>
       </c>
-      <c r="E1" s="31" t="s">
+      <c r="E1" s="32" t="s">
         <v>51</v>
       </c>
-      <c r="F1" s="31" t="s">
+      <c r="F1" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="G1" s="31" t="s">
+      <c r="G1" s="32" t="s">
         <v>53</v>
       </c>
       <c r="H1" s="11" t="s">
@@ -2406,29 +2526,29 @@
       <c r="I1" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="J1" s="31" t="s">
+      <c r="J1" s="32" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="35.4" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="32"/>
+      <c r="A2" s="33"/>
       <c r="B2" s="12" t="s">
         <v>48</v>
       </c>
       <c r="C2" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="33"/>
       <c r="H2" s="12" t="s">
         <v>55</v>
       </c>
       <c r="I2" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="J2" s="32"/>
+      <c r="J2" s="33"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="16">
@@ -3652,7 +3772,7 @@
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="10" spans="6:15" ht="30" x14ac:dyDescent="0.35">
-      <c r="F10" s="31" t="s">
+      <c r="F10" s="32" t="s">
         <v>46</v>
       </c>
       <c r="G10" s="11" t="s">
@@ -3661,16 +3781,16 @@
       <c r="H10" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="I10" s="31" t="s">
+      <c r="I10" s="32" t="s">
         <v>50</v>
       </c>
-      <c r="J10" s="31" t="s">
+      <c r="J10" s="32" t="s">
         <v>51</v>
       </c>
-      <c r="K10" s="31" t="s">
+      <c r="K10" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="L10" s="31" t="s">
+      <c r="L10" s="32" t="s">
         <v>53</v>
       </c>
       <c r="M10" s="11" t="s">
@@ -3679,29 +3799,29 @@
       <c r="N10" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="O10" s="31" t="s">
+      <c r="O10" s="32" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="11" spans="6:15" ht="50" x14ac:dyDescent="0.35">
-      <c r="F11" s="32"/>
+      <c r="F11" s="33"/>
       <c r="G11" s="12" t="s">
         <v>48</v>
       </c>
       <c r="H11" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="I11" s="32"/>
-      <c r="J11" s="32"/>
-      <c r="K11" s="32"/>
-      <c r="L11" s="32"/>
+      <c r="I11" s="33"/>
+      <c r="J11" s="33"/>
+      <c r="K11" s="33"/>
+      <c r="L11" s="33"/>
       <c r="M11" s="12" t="s">
         <v>55</v>
       </c>
       <c r="N11" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="O11" s="32"/>
+      <c r="O11" s="33"/>
     </row>
     <row r="12" spans="6:15" x14ac:dyDescent="0.35">
       <c r="F12" s="16">
@@ -4105,7 +4225,7 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F014ECB5-640D-44E8-8278-F8A28E04C11C}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D988DD2F-F96B-475D-8384-4AA823DA5C06}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
     <ds:schemaRef ds:uri="http://www.boldonjames.com/2008/01/sie/internal/label"/>

</xml_diff>